<commit_message>
1.update kgood abuout xiaxiu
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7270"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="22Q3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>双低备选</t>
   </si>
@@ -25,13 +25,13 @@
     <t>进攻性</t>
   </si>
   <si>
-    <t>其他因素</t>
+    <t>下修评估</t>
   </si>
   <si>
     <t>得分</t>
   </si>
   <si>
-    <t>质押与否</t>
+    <t>担保质押</t>
   </si>
   <si>
     <t>主营业务</t>
@@ -43,16 +43,25 @@
     <t>知名机构</t>
   </si>
   <si>
+    <t>概念题材</t>
+  </si>
+  <si>
+    <t>历史波动</t>
+  </si>
+  <si>
+    <t>业绩预期</t>
+  </si>
+  <si>
+    <t>下修历史</t>
+  </si>
+  <si>
     <t>下修意愿</t>
   </si>
   <si>
-    <t>概念题材</t>
-  </si>
-  <si>
-    <t>历史波动</t>
-  </si>
-  <si>
-    <t>业绩预期</t>
+    <t>现金流/净利</t>
+  </si>
+  <si>
+    <t>资产/负债</t>
   </si>
   <si>
     <t>华源转债</t>
@@ -67,10 +76,19 @@
     <t>李志聪</t>
   </si>
   <si>
+    <t>金属包装</t>
+  </si>
+  <si>
     <t>未下修</t>
   </si>
   <si>
-    <t>金属包装</t>
+    <t>审慎决策</t>
+  </si>
+  <si>
+    <t>2.78/0.45</t>
+  </si>
+  <si>
+    <t>28/12</t>
   </si>
   <si>
     <t>金轮转债</t>
@@ -85,6 +103,12 @@
     <t>氢能</t>
   </si>
   <si>
+    <t>3.65/0.75</t>
+  </si>
+  <si>
+    <t>29/9</t>
+  </si>
+  <si>
     <t>迪贝转债</t>
   </si>
   <si>
@@ -103,6 +127,15 @@
     <t>热泵</t>
   </si>
   <si>
+    <t>23/04/01前不下修</t>
+  </si>
+  <si>
+    <t>2.93/0.32</t>
+  </si>
+  <si>
+    <t>12/4</t>
+  </si>
+  <si>
     <t>合兴转债</t>
   </si>
   <si>
@@ -115,6 +148,15 @@
     <t>环保包装</t>
   </si>
   <si>
+    <t>23/03/07前不下修</t>
+  </si>
+  <si>
+    <t>3.03 /1.23</t>
+  </si>
+  <si>
+    <t>86/50</t>
+  </si>
+  <si>
     <t>奇精转债</t>
   </si>
   <si>
@@ -128,6 +170,15 @@
   </si>
   <si>
     <t>新能源汽车</t>
+  </si>
+  <si>
+    <t>23/04/10前不下修</t>
+  </si>
+  <si>
+    <t>1.62/0.57</t>
+  </si>
+  <si>
+    <t>20/9</t>
   </si>
 </sst>
 </file>
@@ -150,42 +201,31 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <name val="Microsoft YaHei"/>
+      <charset val="0"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Microsoft YaHei"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <name val="Microsoft YaHei"/>
+      <charset val="0"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <name val="Microsoft YaHei"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -281,6 +321,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -518,7 +566,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -544,24 +592,22 @@
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
       <right style="thin">
         <color rgb="FF7F7F7F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
@@ -594,19 +640,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -679,48 +712,51 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -730,43 +766,40 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -775,102 +808,101 @@
     <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1191,379 +1223,431 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:K4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.1666666666667" customWidth="1"/>
-    <col min="2" max="2" width="39.2083333333333" customWidth="1"/>
-    <col min="3" max="3" width="39.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="12.6416666666667" customWidth="1"/>
-    <col min="5" max="5" width="8.325" customWidth="1"/>
-    <col min="6" max="8" width="11.5833333333333" customWidth="1"/>
+    <col min="1" max="1" width="9.34166666666667" customWidth="1"/>
+    <col min="2" max="2" width="26.075" customWidth="1"/>
+    <col min="3" max="3" width="20.4916666666667" customWidth="1"/>
+    <col min="4" max="4" width="12.7416666666667" customWidth="1"/>
+    <col min="5" max="5" width="9.01666666666667" customWidth="1"/>
+    <col min="6" max="6" width="11.275" customWidth="1"/>
+    <col min="7" max="7" width="12.3416666666667" customWidth="1"/>
+    <col min="8" max="8" width="10.7833333333333" customWidth="1"/>
+    <col min="9" max="9" width="12.3416666666667" customWidth="1"/>
+    <col min="10" max="10" width="16.4666666666667" customWidth="1"/>
+    <col min="11" max="12" width="11.8583333333333" customWidth="1"/>
+    <col min="13" max="13" width="8.33333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:12">
+    <row r="1" ht="22.5" customHeight="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="5" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="1" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="16" customHeight="1" spans="1:12">
+    <row r="2" ht="22.5" customHeight="1" spans="1:13">
       <c r="A2" s="1"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="1"/>
+      <c r="J2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1"/>
     </row>
-    <row r="3" ht="28" customHeight="1" spans="1:12">
-      <c r="A3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="10" t="s">
+    <row r="3" ht="41" customHeight="1" spans="1:13">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="10">
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="9">
         <v>2.05</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="9">
+      <c r="H3" s="9"/>
+      <c r="I3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="32" customHeight="1" spans="1:12">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10">
+    <row r="4" ht="36" customHeight="1" spans="1:13">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>0</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>0</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
         <v>1</v>
       </c>
-      <c r="G4" s="10">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:13">
+      <c r="A5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="9">
+        <v>4.2</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" ht="27" customHeight="1" spans="1:13">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9">
         <v>0</v>
       </c>
-      <c r="H4" s="10">
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>4</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" ht="37" customHeight="1" spans="1:13">
+      <c r="A7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="9">
+        <v>3.33</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" ht="37" customHeight="1" spans="1:13">
+      <c r="A8" s="10"/>
+      <c r="B8" s="9">
         <v>2</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="11"/>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>3</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="10"/>
     </row>
-    <row r="5" ht="32" customHeight="1" spans="1:12">
-      <c r="A5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="10" t="s">
+    <row r="9" ht="22.5" customHeight="1" spans="1:13">
+      <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="9">
+        <v>3.47</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="10">
-        <v>4.2</v>
-      </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="9">
-        <v>7</v>
+      <c r="J9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="10">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" ht="24" customHeight="1" spans="1:12">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10">
+    <row r="10" ht="29" customHeight="1" spans="1:13">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9">
         <v>0</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C10" s="9">
         <v>0</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>3</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" ht="22.5" customHeight="1" spans="1:13">
+      <c r="A11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1.3</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" ht="38" customHeight="1" spans="1:13">
+      <c r="A12" s="10"/>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
         <v>0</v>
       </c>
-      <c r="F6" s="10">
+      <c r="D12" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="10">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="H6" s="10">
-        <v>4</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="7" ht="47" customHeight="1" spans="1:12">
-      <c r="A7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="10">
-        <v>3.33</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" ht="24" customHeight="1" spans="1:12">
-      <c r="A8" s="11"/>
-      <c r="B8" s="10">
-        <v>2</v>
-      </c>
-      <c r="C8" s="10">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
+      <c r="G12" s="9">
         <v>1</v>
       </c>
-      <c r="F8" s="10">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9">
         <v>1</v>
       </c>
-      <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="10">
-        <v>3</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" ht="24" customHeight="1" spans="1:12">
-      <c r="A9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="10">
-        <v>3.47</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" ht="26" customHeight="1" spans="1:12">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10">
-        <v>3</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" ht="26" customHeight="1" spans="1:12">
-      <c r="A11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="10">
-        <v>1.3</v>
-      </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" ht="28" customHeight="1" spans="1:12">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10">
-        <v>2</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0</v>
-      </c>
-      <c r="D12" s="10">
-        <v>1</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10">
-        <v>1</v>
-      </c>
-      <c r="G12" s="10">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10">
-        <v>1</v>
-      </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="11"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1.update kgoodlist and selected
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="204">
   <si>
     <t>知名私募/牛散</t>
   </si>
@@ -599,6 +599,36 @@
   </si>
   <si>
     <t>5.4/0.2</t>
+  </si>
+  <si>
+    <t>应急转债</t>
+  </si>
+  <si>
+    <t>无/中国船舶重工</t>
+  </si>
+  <si>
+    <t>专用机械</t>
+  </si>
+  <si>
+    <t>军工</t>
+  </si>
+  <si>
+    <t>6.84/0.019</t>
+  </si>
+  <si>
+    <t>众兴转债</t>
+  </si>
+  <si>
+    <t>无/陶军</t>
+  </si>
+  <si>
+    <t>种植业</t>
+  </si>
+  <si>
+    <t>业绩预增</t>
+  </si>
+  <si>
+    <t>13.4/1.19</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1347,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1340,9 +1370,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="24" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1350,12 +1377,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1736,123 +1757,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="26"/>
+      <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1863,10 +1884,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B57" sqref="$A57:$XFD58"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B59" sqref="$A59:$XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -1936,147 +1957,147 @@
       <c r="H2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" ht="41" customHeight="1" spans="1:13">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="16">
         <v>3.07</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16">
         <v>-0.22</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="16">
         <f>SUM(B4:L4)</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" ht="36" customHeight="1" spans="1:13">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19">
-        <v>0</v>
-      </c>
-      <c r="C4" s="19">
-        <v>0</v>
-      </c>
-      <c r="D4" s="19">
-        <v>0</v>
-      </c>
-      <c r="E4" s="19">
-        <v>1</v>
-      </c>
-      <c r="F4" s="19">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16">
         <v>3</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19">
-        <v>1</v>
-      </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="22">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16">
+        <v>1</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="19">
         <v>-2</v>
       </c>
-      <c r="M4" s="19"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" ht="36" customHeight="1" spans="1:13">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>2.05</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>0.19</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="10">
+      <c r="L5" s="14"/>
+      <c r="M5" s="9">
         <f>SUM(B6:L6)</f>
         <v>4</v>
       </c>
     </row>
     <row r="6" ht="36" customHeight="1" spans="1:13">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
         <v>2</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10">
-        <v>1</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="10"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:13">
       <c r="A7" s="7" t="s">
@@ -2106,7 +2127,7 @@
       <c r="K7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="7">
         <f>SUM(B8:L8)</f>
         <v>7</v>
@@ -2136,7 +2157,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="12"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="7"/>
     </row>
     <row r="9" ht="37" customHeight="1" spans="1:13">
@@ -2171,7 +2192,7 @@
       <c r="K9" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="7">
         <f>SUM(B10:L10)</f>
         <v>7</v>
@@ -2201,262 +2222,262 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="12"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="7"/>
     </row>
     <row r="11" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>3.47</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>0.12</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="10">
+      <c r="L11" s="14"/>
+      <c r="M11" s="9">
         <f>SUM(B12:L12)</f>
         <v>4</v>
       </c>
     </row>
     <row r="12" ht="29" customHeight="1" spans="1:13">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10">
-        <v>0</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0</v>
-      </c>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10">
-        <v>0</v>
-      </c>
-      <c r="F12" s="10">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
         <v>3</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10">
-        <v>1</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="10"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="17">
         <v>1.3</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="17">
         <v>0.19</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="K13" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="10">
+      <c r="L13" s="14"/>
+      <c r="M13" s="9">
         <f>SUM(B14:L14)</f>
         <v>5</v>
       </c>
     </row>
     <row r="14" ht="38" customHeight="1" spans="1:13">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20">
-        <v>1</v>
-      </c>
-      <c r="C14" s="20">
-        <v>0</v>
-      </c>
-      <c r="D14" s="20">
-        <v>1</v>
-      </c>
-      <c r="E14" s="20">
-        <v>1</v>
-      </c>
-      <c r="F14" s="20">
-        <v>1</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20">
-        <v>1</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="10"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17">
+        <v>1</v>
+      </c>
+      <c r="C14" s="17">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17">
+        <v>1</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>3.5</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9">
+      <c r="I15" s="8"/>
+      <c r="J15" s="8">
         <v>0.2</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="9">
+      <c r="L15" s="13"/>
+      <c r="M15" s="8">
         <f>SUM(B16:L16)</f>
         <v>6</v>
       </c>
     </row>
     <row r="16" ht="38" customHeight="1" spans="1:13">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>1</v>
-      </c>
-      <c r="E16" s="9">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
         <v>3</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="9"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="8"/>
     </row>
     <row r="17" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>2.5</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10" t="s">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9">
         <v>0.07</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="10">
+      <c r="L17" s="14"/>
+      <c r="M17" s="9">
         <f>SUM(B18:L18)</f>
         <v>4</v>
       </c>
     </row>
     <row r="18" ht="38" customHeight="1" spans="1:13">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10">
-        <v>1</v>
-      </c>
-      <c r="C18" s="10">
-        <v>0</v>
-      </c>
-      <c r="D18" s="10">
-        <v>0</v>
-      </c>
-      <c r="E18" s="10">
-        <v>0</v>
-      </c>
-      <c r="F18" s="10">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
         <v>2</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10">
-        <v>1</v>
-      </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" ht="22.5" customHeight="1" spans="1:13">
       <c r="A19" s="7" t="s">
@@ -2486,7 +2507,7 @@
       <c r="K19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L19" s="12"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="7">
         <f>SUM(B20:L20)</f>
         <v>6</v>
@@ -2515,137 +2536,137 @@
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="13">
-        <v>1</v>
-      </c>
-      <c r="L20" s="12"/>
+      <c r="K20" s="12">
+        <v>1</v>
+      </c>
+      <c r="L20" s="11"/>
       <c r="M20" s="7"/>
     </row>
     <row r="21" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>3.9</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9" t="s">
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9">
+      <c r="I21" s="8"/>
+      <c r="J21" s="8">
         <v>0.09</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="16"/>
-      <c r="M21" s="9">
+      <c r="L21" s="13"/>
+      <c r="M21" s="8">
         <f>SUM(B22:L22)</f>
         <v>8</v>
       </c>
     </row>
     <row r="22" ht="38" customHeight="1" spans="1:13">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9">
-        <v>1</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0</v>
-      </c>
-      <c r="D22" s="9">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9">
-        <v>1</v>
-      </c>
-      <c r="F22" s="9">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8">
         <v>3</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9">
-        <v>1</v>
-      </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="23">
-        <v>1</v>
-      </c>
-      <c r="L22" s="16"/>
-      <c r="M22" s="9"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="20">
+        <v>1</v>
+      </c>
+      <c r="L22" s="13"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>1.7</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10" t="s">
+      <c r="G23" s="9"/>
+      <c r="H23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10">
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
         <v>0.28</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="L23" s="17"/>
-      <c r="M23" s="10">
+      <c r="L23" s="14"/>
+      <c r="M23" s="9">
         <f>SUM(B24:L24)</f>
         <v>3</v>
       </c>
     </row>
     <row r="24" ht="38" customHeight="1" spans="1:13">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10">
-        <v>0</v>
-      </c>
-      <c r="C24" s="10">
-        <v>0</v>
-      </c>
-      <c r="D24" s="10">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10">
-        <v>1</v>
-      </c>
-      <c r="F24" s="10">
-        <v>1</v>
-      </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10">
-        <v>1</v>
-      </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="9"/>
     </row>
     <row r="25" ht="22.5" customHeight="1" spans="1:13">
       <c r="A25" s="7" t="s">
@@ -2677,7 +2698,7 @@
       <c r="K25" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="L25" s="12"/>
+      <c r="L25" s="11"/>
       <c r="M25" s="7">
         <f>SUM(B26:L26)</f>
         <v>5</v>
@@ -2706,72 +2727,72 @@
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
       <c r="M26" s="7"/>
     </row>
     <row r="27" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="9">
         <v>2.6</v>
       </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10" t="s">
+      <c r="G27" s="9"/>
+      <c r="H27" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10">
+      <c r="I27" s="9"/>
+      <c r="J27" s="9">
         <v>0.21</v>
       </c>
-      <c r="K27" s="10" t="s">
+      <c r="K27" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="10">
+      <c r="L27" s="14"/>
+      <c r="M27" s="9">
         <f t="shared" ref="M27:M31" si="0">SUM(B28:L28)</f>
         <v>4</v>
       </c>
     </row>
     <row r="28" ht="38" customHeight="1" spans="1:13">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10">
-        <v>0</v>
-      </c>
-      <c r="C28" s="10">
-        <v>0</v>
-      </c>
-      <c r="D28" s="10">
-        <v>1</v>
-      </c>
-      <c r="E28" s="10">
-        <v>0</v>
-      </c>
-      <c r="F28" s="10">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0</v>
+      </c>
+      <c r="F28" s="9">
         <v>2</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10">
-        <v>1</v>
-      </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="10"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9">
+        <v>1</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="9"/>
     </row>
     <row r="29" ht="22.5" customHeight="1" spans="1:13">
       <c r="A29" s="7" t="s">
@@ -2803,7 +2824,7 @@
       <c r="K29" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L29" s="12"/>
+      <c r="L29" s="11"/>
       <c r="M29" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2832,880 +2853,998 @@
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="7"/>
     </row>
     <row r="31" ht="36" customHeight="1" spans="1:13">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10" t="s">
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="9">
         <v>3.9</v>
       </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10" t="s">
+      <c r="G31" s="9"/>
+      <c r="H31" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10">
+      <c r="I31" s="9"/>
+      <c r="J31" s="9">
         <v>-0.03</v>
       </c>
-      <c r="K31" s="10" t="s">
+      <c r="K31" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="L31" s="17"/>
-      <c r="M31" s="10">
+      <c r="L31" s="14"/>
+      <c r="M31" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="32" ht="38" customHeight="1" spans="1:13">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10">
-        <v>0</v>
-      </c>
-      <c r="C32" s="10">
-        <v>0</v>
-      </c>
-      <c r="D32" s="10">
-        <v>0</v>
-      </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
-      <c r="F32" s="10">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9">
+        <v>0</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="F32" s="9">
         <v>3</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10">
-        <v>1</v>
-      </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="10"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="9"/>
     </row>
     <row r="33" ht="37" customHeight="1" spans="1:13">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="8">
         <v>6.08</v>
       </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9" t="s">
+      <c r="G33" s="8"/>
+      <c r="H33" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9">
+      <c r="I33" s="8"/>
+      <c r="J33" s="8">
         <v>0.19</v>
       </c>
-      <c r="K33" s="16" t="s">
+      <c r="K33" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="L33" s="16"/>
-      <c r="M33" s="9">
+      <c r="L33" s="13"/>
+      <c r="M33" s="8">
         <f t="shared" ref="M33:M37" si="1">SUM(B34:L34)</f>
         <v>9</v>
       </c>
     </row>
     <row r="34" ht="38" customHeight="1" spans="1:13">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9">
-        <v>0</v>
-      </c>
-      <c r="C34" s="9">
-        <v>0</v>
-      </c>
-      <c r="D34" s="9">
-        <v>1</v>
-      </c>
-      <c r="E34" s="9">
-        <v>1</v>
-      </c>
-      <c r="F34" s="9">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8">
+        <v>0</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0</v>
+      </c>
+      <c r="D34" s="8">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1</v>
+      </c>
+      <c r="F34" s="8">
         <v>6</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9">
-        <v>1</v>
-      </c>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="9"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8">
+        <v>1</v>
+      </c>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="8"/>
     </row>
     <row r="35" ht="36" customHeight="1" spans="1:13">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35" s="8">
         <v>5.16</v>
       </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
+      <c r="G35" s="8"/>
+      <c r="H35" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9">
+      <c r="I35" s="8"/>
+      <c r="J35" s="8">
         <v>0.35</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="L35" s="16"/>
-      <c r="M35" s="9">
+      <c r="L35" s="13"/>
+      <c r="M35" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="36" ht="38" customHeight="1" spans="1:13">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9">
-        <v>0</v>
-      </c>
-      <c r="C36" s="9">
-        <v>0</v>
-      </c>
-      <c r="D36" s="9">
-        <v>1</v>
-      </c>
-      <c r="E36" s="9">
-        <v>1</v>
-      </c>
-      <c r="F36" s="9">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8">
+        <v>1</v>
+      </c>
+      <c r="F36" s="8">
         <v>5</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9">
-        <v>0</v>
-      </c>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="9"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8">
+        <v>0</v>
+      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="8"/>
     </row>
     <row r="37" ht="36" customHeight="1" spans="1:13">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9" t="s">
+      <c r="D37" s="8"/>
+      <c r="E37" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="8">
         <v>6.2</v>
       </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9" t="s">
+      <c r="G37" s="8"/>
+      <c r="H37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9">
+      <c r="I37" s="8"/>
+      <c r="J37" s="8">
         <v>0.28</v>
       </c>
-      <c r="K37" s="9" t="s">
+      <c r="K37" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="L37" s="16"/>
-      <c r="M37" s="9">
+      <c r="L37" s="13"/>
+      <c r="M37" s="8">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="38" ht="38" customHeight="1" spans="1:13">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9">
-        <v>0</v>
-      </c>
-      <c r="C38" s="9">
-        <v>0</v>
-      </c>
-      <c r="D38" s="9">
-        <v>0</v>
-      </c>
-      <c r="E38" s="9">
-        <v>1</v>
-      </c>
-      <c r="F38" s="9">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8">
+        <v>0</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0</v>
+      </c>
+      <c r="D38" s="8">
+        <v>0</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1</v>
+      </c>
+      <c r="F38" s="8">
         <v>6</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9">
-        <v>1</v>
-      </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="9"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8">
+        <v>1</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="8"/>
     </row>
     <row r="39" ht="36" customHeight="1" spans="1:13">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="9">
         <v>5.08</v>
       </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10" t="s">
+      <c r="G39" s="9"/>
+      <c r="H39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10">
+      <c r="I39" s="9"/>
+      <c r="J39" s="9">
         <v>-0.21</v>
       </c>
-      <c r="K39" s="10" t="s">
+      <c r="K39" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="L39" s="17" t="s">
+      <c r="L39" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="9">
         <f t="shared" ref="M39:M43" si="2">SUM(B40:L40)</f>
         <v>8</v>
       </c>
     </row>
     <row r="40" ht="38" customHeight="1" spans="1:13">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10">
-        <v>1</v>
-      </c>
-      <c r="C40" s="10">
-        <v>0</v>
-      </c>
-      <c r="D40" s="10">
-        <v>1</v>
-      </c>
-      <c r="E40" s="10">
-        <v>1</v>
-      </c>
-      <c r="F40" s="10">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9">
+        <v>1</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0</v>
+      </c>
+      <c r="D40" s="9">
+        <v>1</v>
+      </c>
+      <c r="E40" s="9">
+        <v>1</v>
+      </c>
+      <c r="F40" s="9">
         <v>5</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10">
-        <v>1</v>
-      </c>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="18">
+      <c r="G40" s="9"/>
+      <c r="H40" s="9">
+        <v>1</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="15">
         <v>-1</v>
       </c>
-      <c r="M40" s="10"/>
+      <c r="M40" s="9"/>
     </row>
     <row r="41" ht="36" customHeight="1" spans="1:13">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10" t="s">
+      <c r="D41" s="9"/>
+      <c r="E41" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F41" s="9">
         <v>5.06</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10" t="s">
+      <c r="G41" s="9"/>
+      <c r="H41" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10">
+      <c r="I41" s="9"/>
+      <c r="J41" s="9">
         <v>0.33</v>
       </c>
-      <c r="K41" s="10" t="s">
+      <c r="K41" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="L41" s="17"/>
-      <c r="M41" s="10">
+      <c r="L41" s="14"/>
+      <c r="M41" s="9">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
     <row r="42" ht="38" customHeight="1" spans="1:13">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10">
-        <v>1</v>
-      </c>
-      <c r="C42" s="10">
-        <v>0</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10">
-        <v>1</v>
-      </c>
-      <c r="F42" s="10">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9">
+        <v>1</v>
+      </c>
+      <c r="F42" s="9">
         <v>5</v>
       </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10">
-        <v>1</v>
-      </c>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="10"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9">
+        <v>1</v>
+      </c>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="9"/>
     </row>
     <row r="43" ht="36" customHeight="1" spans="1:13">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F43" s="10">
+      <c r="F43" s="9">
         <v>4.23</v>
       </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10" t="s">
+      <c r="G43" s="9"/>
+      <c r="H43" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10">
+      <c r="I43" s="9"/>
+      <c r="J43" s="9">
         <v>0.34</v>
       </c>
-      <c r="K43" s="10" t="s">
+      <c r="K43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="L43" s="17"/>
-      <c r="M43" s="10">
+      <c r="L43" s="14"/>
+      <c r="M43" s="9">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
     <row r="44" ht="38" customHeight="1" spans="1:13">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10">
-        <v>0</v>
-      </c>
-      <c r="C44" s="10">
-        <v>0</v>
-      </c>
-      <c r="D44" s="10">
-        <v>1</v>
-      </c>
-      <c r="E44" s="10">
-        <v>1</v>
-      </c>
-      <c r="F44" s="10">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9">
+        <v>0</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9">
+        <v>1</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1</v>
+      </c>
+      <c r="F44" s="9">
         <v>4</v>
       </c>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10">
-        <v>1</v>
-      </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="10"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="9"/>
     </row>
     <row r="45" ht="36" customHeight="1" spans="1:13">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F45" s="10">
+      <c r="F45" s="9">
         <v>3.8</v>
       </c>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10" t="s">
+      <c r="G45" s="9"/>
+      <c r="H45" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10">
+      <c r="I45" s="9"/>
+      <c r="J45" s="9">
         <v>0.15</v>
       </c>
-      <c r="K45" s="10" t="s">
+      <c r="K45" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L45" s="17"/>
-      <c r="M45" s="10">
+      <c r="L45" s="14"/>
+      <c r="M45" s="9">
         <f t="shared" ref="M45:M49" si="3">SUM(B46:L46)</f>
         <v>6</v>
       </c>
     </row>
     <row r="46" ht="38" customHeight="1" spans="1:13">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10">
-        <v>0</v>
-      </c>
-      <c r="C46" s="10">
-        <v>0</v>
-      </c>
-      <c r="D46" s="10">
-        <v>1</v>
-      </c>
-      <c r="E46" s="10">
-        <v>1</v>
-      </c>
-      <c r="F46" s="10">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9">
+        <v>0</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0</v>
+      </c>
+      <c r="D46" s="9">
+        <v>1</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
         <v>3</v>
       </c>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10">
-        <v>1</v>
-      </c>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="10"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="9"/>
     </row>
     <row r="47" ht="36" customHeight="1" spans="1:13">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10" t="s">
+      <c r="D47" s="9"/>
+      <c r="E47" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F47" s="10">
+      <c r="F47" s="9">
         <v>3.7</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10" t="s">
+      <c r="G47" s="9"/>
+      <c r="H47" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10">
+      <c r="I47" s="9"/>
+      <c r="J47" s="9">
         <v>0.18</v>
       </c>
-      <c r="K47" s="10" t="s">
+      <c r="K47" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="L47" s="17"/>
-      <c r="M47" s="10">
+      <c r="L47" s="14"/>
+      <c r="M47" s="9">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
     <row r="48" ht="38" customHeight="1" spans="1:13">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10">
-        <v>1</v>
-      </c>
-      <c r="C48" s="10">
-        <v>0</v>
-      </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10">
-        <v>1</v>
-      </c>
-      <c r="F48" s="10">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="F48" s="9">
         <v>3</v>
       </c>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10">
-        <v>1</v>
-      </c>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="10"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="9"/>
     </row>
     <row r="49" ht="36" customHeight="1" spans="1:13">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F49" s="9">
         <v>3.6</v>
       </c>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10" t="s">
+      <c r="G49" s="9"/>
+      <c r="H49" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10">
+      <c r="I49" s="9"/>
+      <c r="J49" s="9">
         <v>0.49</v>
       </c>
-      <c r="K49" s="10" t="s">
+      <c r="K49" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="L49" s="17"/>
-      <c r="M49" s="10">
+      <c r="L49" s="14"/>
+      <c r="M49" s="9">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
     <row r="50" ht="38" customHeight="1" spans="1:13">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10">
-        <v>1</v>
-      </c>
-      <c r="C50" s="10">
-        <v>0</v>
-      </c>
-      <c r="D50" s="10">
-        <v>1</v>
-      </c>
-      <c r="E50" s="10">
-        <v>1</v>
-      </c>
-      <c r="F50" s="10">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0</v>
+      </c>
+      <c r="D50" s="9">
+        <v>1</v>
+      </c>
+      <c r="E50" s="9">
+        <v>1</v>
+      </c>
+      <c r="F50" s="9">
         <v>3</v>
       </c>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10">
-        <v>0</v>
-      </c>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="17"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="10"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9">
+        <v>0</v>
+      </c>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="9"/>
     </row>
     <row r="51" ht="36" customHeight="1" spans="1:13">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10" t="s">
+      <c r="C51" s="9"/>
+      <c r="D51" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F51" s="9">
         <v>3.2</v>
       </c>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10" t="s">
+      <c r="G51" s="9"/>
+      <c r="H51" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10">
+      <c r="I51" s="9"/>
+      <c r="J51" s="9">
         <v>-0.05</v>
       </c>
-      <c r="K51" s="10" t="s">
+      <c r="K51" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="L51" s="17"/>
-      <c r="M51" s="10">
+      <c r="L51" s="14"/>
+      <c r="M51" s="9">
         <f t="shared" ref="M51:M55" si="4">SUM(B52:L52)</f>
         <v>7</v>
       </c>
     </row>
     <row r="52" ht="38" customHeight="1" spans="1:13">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10">
-        <v>1</v>
-      </c>
-      <c r="C52" s="10">
-        <v>0</v>
-      </c>
-      <c r="D52" s="10">
-        <v>1</v>
-      </c>
-      <c r="E52" s="10">
-        <v>1</v>
-      </c>
-      <c r="F52" s="10">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9">
+        <v>1</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0</v>
+      </c>
+      <c r="D52" s="9">
+        <v>1</v>
+      </c>
+      <c r="E52" s="9">
+        <v>1</v>
+      </c>
+      <c r="F52" s="9">
         <v>3</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10">
-        <v>1</v>
-      </c>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="17"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="10"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9">
+        <v>1</v>
+      </c>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="9"/>
     </row>
     <row r="53" ht="36" customHeight="1" spans="1:13">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F53" s="9">
         <v>3.07</v>
       </c>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10" t="s">
+      <c r="G53" s="9"/>
+      <c r="H53" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10">
+      <c r="I53" s="9"/>
+      <c r="J53" s="9">
         <v>-0.14</v>
       </c>
-      <c r="K53" s="10" t="s">
+      <c r="K53" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="L53" s="17"/>
-      <c r="M53" s="10">
+      <c r="L53" s="14"/>
+      <c r="M53" s="9">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
     <row r="54" ht="38" customHeight="1" spans="1:13">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10">
-        <v>0</v>
-      </c>
-      <c r="C54" s="10">
-        <v>0</v>
-      </c>
-      <c r="D54" s="10">
-        <v>1</v>
-      </c>
-      <c r="E54" s="10">
-        <v>1</v>
-      </c>
-      <c r="F54" s="10">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9">
+        <v>0</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0</v>
+      </c>
+      <c r="D54" s="9">
+        <v>1</v>
+      </c>
+      <c r="E54" s="9">
+        <v>1</v>
+      </c>
+      <c r="F54" s="9">
         <v>3</v>
       </c>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10">
-        <v>1</v>
-      </c>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="10"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9">
+        <v>1</v>
+      </c>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="9"/>
     </row>
     <row r="55" ht="36" customHeight="1" spans="1:13">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F55" s="7">
         <v>5.9</v>
       </c>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8" t="s">
+      <c r="G55" s="7"/>
+      <c r="H55" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8">
+      <c r="I55" s="7"/>
+      <c r="J55" s="7">
         <v>-0.03</v>
       </c>
-      <c r="K55" s="8" t="s">
+      <c r="K55" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="L55" s="14"/>
-      <c r="M55" s="8">
+      <c r="L55" s="11"/>
+      <c r="M55" s="7">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
     <row r="56" ht="38" customHeight="1" spans="1:13">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8">
-        <v>1</v>
-      </c>
-      <c r="C56" s="8">
-        <v>0</v>
-      </c>
-      <c r="D56" s="8">
-        <v>1</v>
-      </c>
-      <c r="E56" s="8">
-        <v>1</v>
-      </c>
-      <c r="F56" s="8">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7">
+        <v>1</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0</v>
+      </c>
+      <c r="D56" s="7">
+        <v>1</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1</v>
+      </c>
+      <c r="F56" s="7">
         <v>5</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8">
-        <v>1</v>
-      </c>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="15"/>
-      <c r="M56" s="8"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7">
+        <v>1</v>
+      </c>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="7"/>
     </row>
     <row r="57" ht="36" customHeight="1" spans="1:13">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8" t="s">
+      <c r="D57" s="7"/>
+      <c r="E57" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F57" s="7">
         <v>3.7</v>
       </c>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8" t="s">
+      <c r="G57" s="7"/>
+      <c r="H57" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8">
+      <c r="I57" s="7"/>
+      <c r="J57" s="7">
         <v>-0.06</v>
       </c>
-      <c r="K57" s="8" t="s">
+      <c r="K57" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="L57" s="14"/>
-      <c r="M57" s="8">
-        <f>SUM(B58:L58)</f>
+      <c r="L57" s="11"/>
+      <c r="M57" s="7">
+        <f t="shared" ref="M57:M61" si="5">SUM(B58:L58)</f>
         <v>6</v>
       </c>
     </row>
     <row r="58" ht="38" customHeight="1" spans="1:13">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8">
-        <v>1</v>
-      </c>
-      <c r="C58" s="8">
-        <v>0</v>
-      </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8">
-        <v>1</v>
-      </c>
-      <c r="F58" s="8">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7">
+        <v>1</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7">
         <v>3</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8">
-        <v>1</v>
-      </c>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="8"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7">
+        <v>1</v>
+      </c>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="7"/>
+    </row>
+    <row r="59" ht="36" customHeight="1" spans="1:13">
+      <c r="A59" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F59" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7">
+        <v>-0.58</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="L59" s="11"/>
+      <c r="M59" s="7">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" ht="38" customHeight="1" spans="1:13">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7">
+        <v>1</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7">
+        <v>2</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7">
+        <v>1</v>
+      </c>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="7"/>
+    </row>
+    <row r="61" ht="36" customHeight="1" spans="1:13">
+      <c r="A61" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F61" s="7">
+        <v>3</v>
+      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="L61" s="11"/>
+      <c r="M61" s="7">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" ht="38" customHeight="1" spans="1:13">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7">
+        <v>0</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7">
+        <v>3</v>
+      </c>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7">
+        <v>1</v>
+      </c>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="66">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:I1"/>
@@ -3739,6 +3878,8 @@
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A61:A62"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="M5:M6"/>
@@ -3768,6 +3909,8 @@
     <mergeCell ref="M53:M54"/>
     <mergeCell ref="M55:M56"/>
     <mergeCell ref="M57:M58"/>
+    <mergeCell ref="M59:M60"/>
+    <mergeCell ref="M61:M62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3777,10 +3920,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15:M16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="$A13:$XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -3850,16 +3993,16 @@
       <c r="H2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="1"/>
@@ -3892,7 +4035,7 @@
       <c r="K3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="7">
         <f>SUM(B4:L4)</f>
         <v>7</v>
@@ -3922,7 +4065,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="12"/>
+      <c r="L4" s="11"/>
       <c r="M4" s="7"/>
     </row>
     <row r="5" ht="37" customHeight="1" spans="1:13">
@@ -3957,7 +4100,7 @@
       <c r="K5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L5" s="12"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="7">
         <f>SUM(B6:L6)</f>
         <v>7</v>
@@ -3987,7 +4130,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="12"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="7"/>
     </row>
     <row r="7" ht="22.5" customHeight="1" spans="1:13">
@@ -4018,7 +4161,7 @@
       <c r="K7" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="7">
         <f>SUM(B8:L8)</f>
         <v>6</v>
@@ -4047,10 +4190,10 @@
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="13">
-        <v>1</v>
-      </c>
-      <c r="L8" s="12"/>
+      <c r="K8" s="12">
+        <v>1</v>
+      </c>
+      <c r="L8" s="11"/>
       <c r="M8" s="7"/>
     </row>
     <row r="9" ht="22.5" customHeight="1" spans="1:13">
@@ -4083,7 +4226,7 @@
       <c r="K9" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="7">
         <f t="shared" ref="M9:M13" si="0">SUM(B10:L10)</f>
         <v>5</v>
@@ -4112,8 +4255,8 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="7"/>
     </row>
     <row r="11" ht="22.5" customHeight="1" spans="1:13">
@@ -4146,7 +4289,7 @@
       <c r="K11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L11" s="12"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4175,483 +4318,475 @@
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="7"/>
     </row>
     <row r="13" ht="36" customHeight="1" spans="1:13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>5.9</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7">
         <v>-0.03</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="8">
+      <c r="L13" s="11"/>
+      <c r="M13" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="14" ht="38" customHeight="1" spans="1:13">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
         <v>5</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="8"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" ht="36" customHeight="1" spans="1:13">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>3.7</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8">
+      <c r="I15" s="7"/>
+      <c r="J15" s="7">
         <v>-0.06</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="8">
-        <f>SUM(B16:L16)</f>
+      <c r="L15" s="11"/>
+      <c r="M15" s="7">
+        <f t="shared" ref="M15:M19" si="1">SUM(B16:L16)</f>
         <v>6</v>
       </c>
     </row>
     <row r="16" ht="38" customHeight="1" spans="1:13">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8">
-        <v>1</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7">
         <v>3</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8">
-        <v>1</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="8"/>
-    </row>
-    <row r="17" ht="37" customHeight="1" spans="1:13">
-      <c r="A17" s="9" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" ht="36" customHeight="1" spans="1:13">
+      <c r="A17" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7">
+        <v>-0.58</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" ht="38" customHeight="1" spans="1:13">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" ht="36" customHeight="1" spans="1:13">
+      <c r="A19" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19" s="7">
+        <v>3</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" ht="38" customHeight="1" spans="1:13">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="7"/>
+    </row>
+    <row r="21" ht="37" customHeight="1" spans="1:13">
+      <c r="A21" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F21" s="8">
         <v>6.08</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9">
+      <c r="I21" s="8"/>
+      <c r="J21" s="8">
         <v>0.19</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="K21" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="9">
-        <f>SUM(B18:L18)</f>
+      <c r="L21" s="13"/>
+      <c r="M21" s="8">
+        <f>SUM(B22:L22)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="18" ht="38" customHeight="1" spans="1:13">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9">
-        <v>0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9">
+    <row r="22" ht="38" customHeight="1" spans="1:13">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8">
         <v>6</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9">
-        <v>1</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" ht="36" customHeight="1" spans="1:13">
-      <c r="A19" s="10" t="s">
+      <c r="G22" s="8"/>
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" ht="36" customHeight="1" spans="1:13">
+      <c r="A23" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F23" s="9">
         <v>5.06</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10" t="s">
+      <c r="G23" s="9"/>
+      <c r="H23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10">
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
         <v>0.33</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K23" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="L19" s="17"/>
-      <c r="M19" s="10">
-        <f>SUM(B20:L20)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" ht="38" customHeight="1" spans="1:13">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10">
-        <v>1</v>
-      </c>
-      <c r="C20" s="10">
-        <v>0</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10">
-        <v>1</v>
-      </c>
-      <c r="F20" s="10">
-        <v>5</v>
-      </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10">
-        <v>1</v>
-      </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="10"/>
-    </row>
-    <row r="21" ht="36" customHeight="1" spans="1:13">
-      <c r="A21" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F21" s="9">
-        <v>6.2</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9">
-        <v>0.28</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="L21" s="16"/>
-      <c r="M21" s="9">
-        <f>SUM(B22:L22)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" ht="38" customHeight="1" spans="1:13">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0</v>
-      </c>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-      <c r="E22" s="9">
-        <v>1</v>
-      </c>
-      <c r="F22" s="9">
-        <v>6</v>
-      </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9">
-        <v>1</v>
-      </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="9"/>
-    </row>
-    <row r="23" ht="36" customHeight="1" spans="1:13">
-      <c r="A23" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" s="10">
-        <v>5.08</v>
-      </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10">
-        <v>-0.21</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="M23" s="10">
+      <c r="L23" s="14"/>
+      <c r="M23" s="9">
         <f>SUM(B24:L24)</f>
         <v>8</v>
       </c>
     </row>
     <row r="24" ht="38" customHeight="1" spans="1:13">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10">
-        <v>0</v>
-      </c>
-      <c r="D24" s="10">
-        <v>1</v>
-      </c>
-      <c r="E24" s="10">
-        <v>1</v>
-      </c>
-      <c r="F24" s="10">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9">
         <v>5</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10">
-        <v>1</v>
-      </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="18">
-        <v>-1</v>
-      </c>
-      <c r="M24" s="10"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="9"/>
     </row>
     <row r="25" ht="36" customHeight="1" spans="1:13">
-      <c r="A25" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="F25" s="10">
-        <v>3.2</v>
-      </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10" t="s">
+      <c r="A25" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" s="8">
+        <v>6.2</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10">
-        <v>-0.05</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="L25" s="17"/>
-      <c r="M25" s="10">
+      <c r="I25" s="8"/>
+      <c r="J25" s="8">
+        <v>0.28</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="L25" s="13"/>
+      <c r="M25" s="8">
         <f>SUM(B26:L26)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" ht="38" customHeight="1" spans="1:13">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10">
-        <v>1</v>
-      </c>
-      <c r="C26" s="10">
-        <v>0</v>
-      </c>
-      <c r="D26" s="10">
-        <v>1</v>
-      </c>
-      <c r="E26" s="10">
-        <v>1</v>
-      </c>
-      <c r="F26" s="10">
-        <v>3</v>
-      </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10">
-        <v>1</v>
-      </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8">
+        <v>0</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="8">
+        <v>6</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8">
+        <v>1</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="8"/>
     </row>
     <row r="27" ht="36" customHeight="1" spans="1:13">
       <c r="A27" s="9" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="F27" s="9">
-        <v>5.16</v>
+        <v>5.08</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9">
-        <v>0.35</v>
+        <v>-0.21</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="L27" s="16"/>
+        <v>148</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>149</v>
+      </c>
       <c r="M27" s="9">
         <f>SUM(B28:L28)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" ht="38" customHeight="1" spans="1:13">
       <c r="A28" s="9"/>
       <c r="B28" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="9">
         <v>0</v>
@@ -4667,451 +4802,577 @@
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="15">
+        <v>-1</v>
+      </c>
       <c r="M28" s="9"/>
     </row>
     <row r="29" ht="36" customHeight="1" spans="1:13">
-      <c r="A29" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F29" s="10">
-        <v>4.23</v>
-      </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10" t="s">
+      <c r="A29" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" s="9">
+        <v>3.2</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10">
-        <v>0.34</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="L29" s="17"/>
-      <c r="M29" s="10">
+      <c r="I29" s="9"/>
+      <c r="J29" s="9">
+        <v>-0.05</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="L29" s="14"/>
+      <c r="M29" s="9">
         <f>SUM(B30:L30)</f>
         <v>7</v>
       </c>
     </row>
     <row r="30" ht="38" customHeight="1" spans="1:13">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10">
-        <v>0</v>
-      </c>
-      <c r="C30" s="10">
-        <v>0</v>
-      </c>
-      <c r="D30" s="10">
-        <v>1</v>
-      </c>
-      <c r="E30" s="10">
-        <v>1</v>
-      </c>
-      <c r="F30" s="10">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>1</v>
+      </c>
+      <c r="E30" s="9">
+        <v>1</v>
+      </c>
+      <c r="F30" s="9">
+        <v>3</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9">
+        <v>1</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" ht="36" customHeight="1" spans="1:13">
+      <c r="A31" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="8">
+        <v>5.16</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L31" s="13"/>
+      <c r="M31" s="8">
+        <f>SUM(B32:L32)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" ht="38" customHeight="1" spans="1:13">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8">
+        <v>5</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8">
+        <v>0</v>
+      </c>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" ht="36" customHeight="1" spans="1:13">
+      <c r="A33" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F33" s="9">
+        <v>4.23</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9">
+        <v>0.34</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L33" s="14"/>
+      <c r="M33" s="9">
+        <f>SUM(B34:L34)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" ht="38" customHeight="1" spans="1:13">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9">
+        <v>0</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <v>1</v>
+      </c>
+      <c r="E34" s="9">
+        <v>1</v>
+      </c>
+      <c r="F34" s="9">
         <v>4</v>
       </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10">
-        <v>1</v>
-      </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="10"/>
-    </row>
-    <row r="31" ht="22.5" customHeight="1" spans="1:13">
-      <c r="A31" s="9" t="s">
+      <c r="G34" s="9"/>
+      <c r="H34" s="9">
+        <v>1</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="9"/>
+    </row>
+    <row r="35" ht="22.5" customHeight="1" spans="1:13">
+      <c r="A35" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D35" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F35" s="8">
         <v>3.5</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
+      <c r="G35" s="8"/>
+      <c r="H35" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9">
+      <c r="I35" s="8"/>
+      <c r="J35" s="8">
         <v>0.2</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="K35" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="L31" s="16"/>
-      <c r="M31" s="9">
-        <f>SUM(B32:L32)</f>
+      <c r="L35" s="13"/>
+      <c r="M35" s="8">
+        <f>SUM(B36:L36)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="32" ht="38" customHeight="1" spans="1:13">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9">
-        <v>0</v>
-      </c>
-      <c r="C32" s="9">
-        <v>0</v>
-      </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
-        <v>1</v>
-      </c>
-      <c r="F32" s="9">
+    <row r="36" ht="38" customHeight="1" spans="1:13">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8">
+        <v>1</v>
+      </c>
+      <c r="F36" s="8">
         <v>3</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9">
-        <v>1</v>
-      </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="9"/>
-    </row>
-    <row r="33" ht="36" customHeight="1" spans="1:13">
-      <c r="A33" s="10" t="s">
+      <c r="G36" s="8"/>
+      <c r="H36" s="8">
+        <v>1</v>
+      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" ht="36" customHeight="1" spans="1:13">
+      <c r="A37" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F37" s="9">
         <v>3.8</v>
       </c>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10" t="s">
+      <c r="G37" s="9"/>
+      <c r="H37" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10">
+      <c r="I37" s="9"/>
+      <c r="J37" s="9">
         <v>0.15</v>
       </c>
-      <c r="K33" s="10" t="s">
+      <c r="K37" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L33" s="17"/>
-      <c r="M33" s="10">
-        <f t="shared" ref="M33:M37" si="1">SUM(B34:L34)</f>
+      <c r="L37" s="14"/>
+      <c r="M37" s="9">
+        <f t="shared" ref="M37:M41" si="2">SUM(B38:L38)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="34" ht="38" customHeight="1" spans="1:13">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10">
-        <v>0</v>
-      </c>
-      <c r="C34" s="10">
-        <v>0</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10">
-        <v>1</v>
-      </c>
-      <c r="F34" s="10">
+    <row r="38" ht="38" customHeight="1" spans="1:13">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9">
+        <v>0</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1</v>
+      </c>
+      <c r="F38" s="9">
         <v>3</v>
       </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10">
-        <v>1</v>
-      </c>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="10"/>
-    </row>
-    <row r="35" ht="36" customHeight="1" spans="1:13">
-      <c r="A35" s="10" t="s">
+      <c r="G38" s="9"/>
+      <c r="H38" s="9">
+        <v>1</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="9"/>
+    </row>
+    <row r="39" ht="36" customHeight="1" spans="1:13">
+      <c r="A39" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10" t="s">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F39" s="9">
         <v>3.7</v>
       </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10" t="s">
+      <c r="G39" s="9"/>
+      <c r="H39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10">
+      <c r="I39" s="9"/>
+      <c r="J39" s="9">
         <v>0.18</v>
       </c>
-      <c r="K35" s="10" t="s">
+      <c r="K39" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="L35" s="17"/>
-      <c r="M35" s="10">
-        <f t="shared" si="1"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="9">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="36" ht="38" customHeight="1" spans="1:13">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10">
-        <v>1</v>
-      </c>
-      <c r="C36" s="10">
-        <v>0</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10">
-        <v>1</v>
-      </c>
-      <c r="F36" s="10">
+    <row r="40" ht="38" customHeight="1" spans="1:13">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9">
+        <v>1</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9">
+        <v>1</v>
+      </c>
+      <c r="F40" s="9">
         <v>3</v>
       </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10">
-        <v>1</v>
-      </c>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="10"/>
-    </row>
-    <row r="37" ht="36" customHeight="1" spans="1:13">
-      <c r="A37" s="10" t="s">
+      <c r="G40" s="9"/>
+      <c r="H40" s="9">
+        <v>1</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="9"/>
+    </row>
+    <row r="41" ht="36" customHeight="1" spans="1:13">
+      <c r="A41" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D41" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F41" s="9">
         <v>3.6</v>
       </c>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10" t="s">
+      <c r="G41" s="9"/>
+      <c r="H41" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10">
+      <c r="I41" s="9"/>
+      <c r="J41" s="9">
         <v>0.49</v>
       </c>
-      <c r="K37" s="10" t="s">
+      <c r="K41" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="L37" s="17"/>
-      <c r="M37" s="10">
-        <f t="shared" si="1"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="9">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="38" ht="38" customHeight="1" spans="1:13">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10">
-        <v>1</v>
-      </c>
-      <c r="C38" s="10">
-        <v>0</v>
-      </c>
-      <c r="D38" s="10">
-        <v>1</v>
-      </c>
-      <c r="E38" s="10">
-        <v>1</v>
-      </c>
-      <c r="F38" s="10">
+    <row r="42" ht="38" customHeight="1" spans="1:13">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0</v>
+      </c>
+      <c r="D42" s="9">
+        <v>1</v>
+      </c>
+      <c r="E42" s="9">
+        <v>1</v>
+      </c>
+      <c r="F42" s="9">
         <v>3</v>
       </c>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10">
-        <v>0</v>
-      </c>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="10"/>
-    </row>
-    <row r="39" ht="36" customHeight="1" spans="1:13">
-      <c r="A39" s="10" t="s">
+      <c r="G42" s="9"/>
+      <c r="H42" s="9">
+        <v>0</v>
+      </c>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="9"/>
+    </row>
+    <row r="43" ht="36" customHeight="1" spans="1:13">
+      <c r="A43" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D43" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F43" s="9">
         <v>3.07</v>
       </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10" t="s">
+      <c r="G43" s="9"/>
+      <c r="H43" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10">
+      <c r="I43" s="9"/>
+      <c r="J43" s="9">
         <v>-0.14</v>
       </c>
-      <c r="K39" s="10" t="s">
+      <c r="K43" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="L39" s="17"/>
-      <c r="M39" s="10">
-        <f>SUM(B40:L40)</f>
+      <c r="L43" s="14"/>
+      <c r="M43" s="9">
+        <f>SUM(B44:L44)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="40" ht="38" customHeight="1" spans="1:13">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10">
-        <v>0</v>
-      </c>
-      <c r="C40" s="10">
-        <v>0</v>
-      </c>
-      <c r="D40" s="10">
-        <v>1</v>
-      </c>
-      <c r="E40" s="10">
-        <v>1</v>
-      </c>
-      <c r="F40" s="10">
+    <row r="44" ht="38" customHeight="1" spans="1:13">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9">
+        <v>0</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9">
+        <v>1</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1</v>
+      </c>
+      <c r="F44" s="9">
         <v>3</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10">
-        <v>1</v>
-      </c>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="10"/>
-    </row>
-    <row r="41" ht="36" customHeight="1" spans="1:13">
-      <c r="A41" s="10" t="s">
+      <c r="G44" s="9"/>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="9"/>
+    </row>
+    <row r="45" ht="36" customHeight="1" spans="1:13">
+      <c r="A45" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10" t="s">
+      <c r="D45" s="9"/>
+      <c r="E45" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F45" s="9">
         <v>3.9</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10" t="s">
+      <c r="G45" s="9"/>
+      <c r="H45" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10">
+      <c r="I45" s="9"/>
+      <c r="J45" s="9">
         <v>-0.03</v>
       </c>
-      <c r="K41" s="10" t="s">
+      <c r="K45" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="L41" s="17"/>
-      <c r="M41" s="10">
-        <f>SUM(B42:L42)</f>
+      <c r="L45" s="14"/>
+      <c r="M45" s="9">
+        <f>SUM(B46:L46)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="42" ht="38" customHeight="1" spans="1:13">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10">
-        <v>0</v>
-      </c>
-      <c r="C42" s="10">
-        <v>0</v>
-      </c>
-      <c r="D42" s="10">
-        <v>0</v>
-      </c>
-      <c r="E42" s="10">
-        <v>1</v>
-      </c>
-      <c r="F42" s="10">
+    <row r="46" ht="38" customHeight="1" spans="1:13">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9">
+        <v>0</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
         <v>3</v>
       </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10">
-        <v>1</v>
-      </c>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="10"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="50">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:I1"/>
@@ -5137,6 +5398,8 @@
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="M5:M6"/>
@@ -5158,6 +5421,8 @@
     <mergeCell ref="M37:M38"/>
     <mergeCell ref="M39:M40"/>
     <mergeCell ref="M41:M42"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="M45:M46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1.update for new akshare with Anaconda3-2023.03
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -1886,7 +1886,7 @@
   <sheetPr/>
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A52" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A48" workbookViewId="0">
       <selection activeCell="B59" sqref="$A59:$XFD62"/>
     </sheetView>
   </sheetViews>
@@ -3922,8 +3922,8 @@
   <sheetPr/>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="$A13:$XFD16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B19" sqref="$A19:$XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
1.add some in kgooglist
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="7140" activeTab="3"/>
+    <workbookView windowWidth="18530" windowHeight="7270" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="227">
   <si>
     <t>知名私募/牛散</t>
   </si>
@@ -663,12 +663,48 @@
   </si>
   <si>
     <t>4.69/0.43</t>
+  </si>
+  <si>
+    <t>银微转债</t>
+  </si>
+  <si>
+    <t>半导体</t>
+  </si>
+  <si>
+    <t>汽车半导体</t>
+  </si>
+  <si>
+    <t>2..04/0.3</t>
+  </si>
+  <si>
+    <t>英力转债</t>
+  </si>
+  <si>
+    <t>消费电子</t>
+  </si>
+  <si>
+    <t>1.68/-0.2</t>
+  </si>
+  <si>
+    <t>丰山转债</t>
+  </si>
+  <si>
+    <t>抵押担保</t>
+  </si>
+  <si>
+    <t>农药</t>
+  </si>
+  <si>
+    <t>钠电池</t>
+  </si>
+  <si>
+    <t>3.57/-0.17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -736,6 +772,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -749,6 +813,14 @@
       <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -793,21 +865,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -845,28 +902,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -929,7 +965,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -941,7 +983,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -965,18 +1055,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -989,31 +1067,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1037,19 +1091,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,12 +1110,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1236,272 +1272,272 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="24" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="24" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="24" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="24" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="31" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="17" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="17" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="24" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="24" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1920,8 +1956,8 @@
   <sheetPr/>
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:M6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B41" sqref="$A41:$XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -3956,7 +3992,7 @@
   <sheetPr/>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A37" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B19" sqref="$A19:$XFD20"/>
     </sheetView>
   </sheetViews>
@@ -5466,13 +5502,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="9.33333333333333" customWidth="1"/>
     <col min="2" max="2" width="33.8333333333333" customWidth="1"/>
@@ -5585,7 +5621,7 @@
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="7">
-        <f>SUM(B4:L4)</f>
+        <f t="shared" ref="M3:M7" si="0">SUM(B4:L4)</f>
         <v>6</v>
       </c>
     </row>
@@ -5648,7 +5684,7 @@
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="7">
-        <f>SUM(B6:L6)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -5679,8 +5715,185 @@
       <c r="L6" s="9"/>
       <c r="M6" s="7"/>
     </row>
+    <row r="7" ht="36" customHeight="1" spans="1:13">
+      <c r="A7" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" ht="36" customHeight="1" spans="1:13">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" ht="36" customHeight="1" spans="1:13">
+      <c r="A9" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="7">
+        <f>SUM(B10:L10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" ht="36" customHeight="1" spans="1:13">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" ht="36" customHeight="1" spans="1:13">
+      <c r="A11" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7">
+        <v>-0.12</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="7">
+        <f>SUM(B12:L12)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" ht="36" customHeight="1" spans="1:13">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="16">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:I1"/>
@@ -5688,9 +5901,15 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1.add crash column for result
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="258">
   <si>
     <t>知名私募/牛散</t>
   </si>
@@ -749,6 +749,63 @@
   </si>
   <si>
     <t>8.48/1.5</t>
+  </si>
+  <si>
+    <t>海波转债</t>
+  </si>
+  <si>
+    <t>张海波</t>
+  </si>
+  <si>
+    <t>桥梁设计</t>
+  </si>
+  <si>
+    <t>一带一路</t>
+  </si>
+  <si>
+    <t>0.7/0.062</t>
+  </si>
+  <si>
+    <t>乐歌转债</t>
+  </si>
+  <si>
+    <t>项乐宏</t>
+  </si>
+  <si>
+    <t>家用轻工</t>
+  </si>
+  <si>
+    <t>智能家居</t>
+  </si>
+  <si>
+    <t>15.16/5.17</t>
+  </si>
+  <si>
+    <t>法兰转债</t>
+  </si>
+  <si>
+    <t>质押担保/陶峰华</t>
+  </si>
+  <si>
+    <t>起重机</t>
+  </si>
+  <si>
+    <t>换电</t>
+  </si>
+  <si>
+    <t>3.09/1.39</t>
+  </si>
+  <si>
+    <t>银信转债</t>
+  </si>
+  <si>
+    <t>詹立雄</t>
+  </si>
+  <si>
+    <t>软件</t>
+  </si>
+  <si>
+    <t>5.53/1.19</t>
   </si>
 </sst>
 </file>
@@ -2006,8 +2063,8 @@
   <sheetPr/>
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B41" sqref="$A41:$XFD42"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -6036,8 +6093,8 @@
   <sheetPr/>
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -6248,29 +6305,56 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" ht="36" customHeight="1" spans="1:13">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>241</v>
+      </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" s="7">
+        <v>3.16</v>
+      </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="J7" s="7">
+        <v>-0.05</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>243</v>
+      </c>
       <c r="L7" s="9"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="7">
+        <f>SUM(B8:L8)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="8" ht="36" customHeight="1" spans="1:13">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>3</v>
+      </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -6278,29 +6362,62 @@
       <c r="M8" s="7"/>
     </row>
     <row r="9" ht="36" customHeight="1" spans="1:13">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2.7</v>
+      </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="J9" s="7">
+        <v>0.27</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>248</v>
+      </c>
       <c r="L9" s="9"/>
-      <c r="M9" s="7"/>
+      <c r="M9" s="7">
+        <f>SUM(B10:L10)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="10" ht="36" customHeight="1" spans="1:13">
       <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -6308,29 +6425,56 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" ht="36" customHeight="1" spans="1:13">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>251</v>
+      </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2.8</v>
+      </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="J11" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>253</v>
+      </c>
       <c r="L11" s="9"/>
-      <c r="M11" s="7"/>
+      <c r="M11" s="7">
+        <f>SUM(B12:L12)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="12" ht="36" customHeight="1" spans="1:13">
       <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -6338,29 +6482,58 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" ht="36" customHeight="1" spans="1:13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2.5</v>
+      </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="J13" s="7">
+        <v>0.14</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>257</v>
+      </c>
       <c r="L13" s="9"/>
-      <c r="M13" s="7"/>
+      <c r="M13" s="7">
+        <f>SUM(B14:L14)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="14" ht="36" customHeight="1" spans="1:13">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>

</xml_diff>

<commit_message>
1.add kairun in kgoodlist
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="7140"/>
+    <workbookView windowWidth="18350" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="205">
   <si>
     <t>知名私募/牛散</t>
   </si>
@@ -635,6 +635,15 @@
   </si>
   <si>
     <t>威唐转债</t>
+  </si>
+  <si>
+    <t>开润转债</t>
+  </si>
+  <si>
+    <t>箱包</t>
+  </si>
+  <si>
+    <t>小米</t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1796,7 @@
   <sheetPr/>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1959,10 +1968,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -2167,7 +2176,7 @@
       </c>
       <c r="P5" s="10">
         <f>SUM(B6:O6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" ht="36" customHeight="1" spans="1:16">
@@ -2195,9 +2204,7 @@
         <v>63</v>
       </c>
       <c r="L6" s="10"/>
-      <c r="M6" s="10">
-        <v>-1</v>
-      </c>
+      <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="19">
         <v>-1</v>
@@ -2249,7 +2256,7 @@
       <c r="O7" s="21"/>
       <c r="P7" s="10">
         <f>SUM(B8:O8)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" ht="37" customHeight="1" spans="1:16">
@@ -2275,9 +2282,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="21"/>
       <c r="L8" s="11"/>
-      <c r="M8" s="11">
-        <v>-1</v>
-      </c>
+      <c r="M8" s="11"/>
       <c r="N8" s="11">
         <v>1</v>
       </c>
@@ -2388,7 +2393,7 @@
       <c r="O11" s="21"/>
       <c r="P11" s="10">
         <f>SUM(B12:O12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" ht="38" customHeight="1" spans="1:16">
@@ -2416,9 +2421,7 @@
       <c r="J12" s="23"/>
       <c r="K12" s="21"/>
       <c r="L12" s="11"/>
-      <c r="M12" s="11">
-        <v>-1</v>
-      </c>
+      <c r="M12" s="11"/>
       <c r="N12" s="11">
         <v>-1</v>
       </c>
@@ -2529,7 +2532,7 @@
       <c r="O15" s="21"/>
       <c r="P15" s="10">
         <f>SUM(B16:O16)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" ht="38" customHeight="1" spans="1:16">
@@ -2555,9 +2558,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="11"/>
-      <c r="M16" s="11">
-        <v>-1</v>
-      </c>
+      <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="23"/>
       <c r="P16" s="10"/>
@@ -3430,7 +3431,7 @@
       <c r="O41" s="21"/>
       <c r="P41" s="10">
         <f>SUM(B42:O42)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" ht="38" customHeight="1" spans="1:16">
@@ -3456,9 +3457,7 @@
       <c r="J42" s="21"/>
       <c r="K42" s="23"/>
       <c r="L42" s="11"/>
-      <c r="M42" s="11">
-        <v>-1</v>
-      </c>
+      <c r="M42" s="11"/>
       <c r="N42" s="11">
         <v>1</v>
       </c>
@@ -4499,7 +4498,7 @@
       </c>
       <c r="O75" s="21"/>
       <c r="P75" s="10">
-        <f>SUM(B76:O76)</f>
+        <f t="shared" ref="P75:P79" si="7">SUM(B76:O76)</f>
         <v>4</v>
       </c>
     </row>
@@ -4569,7 +4568,7 @@
       <c r="N77" s="21"/>
       <c r="O77" s="21"/>
       <c r="P77" s="10">
-        <f>SUM(B78:O78)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
@@ -4599,8 +4598,78 @@
       <c r="O78" s="21"/>
       <c r="P78" s="10"/>
     </row>
+    <row r="79" customFormat="1" ht="36" customHeight="1" spans="1:16">
+      <c r="A79" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B79" s="11"/>
+      <c r="C79" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F79" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H79" s="11">
+        <v>0.3264</v>
+      </c>
+      <c r="I79" s="11">
+        <v>59.7197</v>
+      </c>
+      <c r="J79" s="11">
+        <v>11.45</v>
+      </c>
+      <c r="K79" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L79" s="22">
+        <v>46017</v>
+      </c>
+      <c r="M79" s="21" t="str">
+        <f ca="1">DATEDIF(TODAY(),L79,"y")&amp;"年"&amp;DATEDIF(TODAY(),L79,"ym")&amp;"月"</f>
+        <v>1年5月</v>
+      </c>
+      <c r="N79" s="21"/>
+      <c r="O79" s="21"/>
+      <c r="P79" s="10">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" customFormat="1" ht="36" customHeight="1" spans="1:16">
+      <c r="A80" s="11"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11">
+        <v>1</v>
+      </c>
+      <c r="E80" s="11">
+        <v>1</v>
+      </c>
+      <c r="F80" s="11">
+        <v>1</v>
+      </c>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="23"/>
+      <c r="L80" s="22"/>
+      <c r="M80" s="21"/>
+      <c r="N80" s="21"/>
+      <c r="O80" s="21"/>
+      <c r="P80" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="82">
+  <mergeCells count="84">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -4644,6 +4713,7 @@
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="A75:A76"/>
     <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A80"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="P5:P6"/>
@@ -4683,6 +4753,7 @@
     <mergeCell ref="P73:P74"/>
     <mergeCell ref="P75:P76"/>
     <mergeCell ref="P77:P78"/>
+    <mergeCell ref="P79:P80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1.fix some in kgoodlist
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="205">
   <si>
     <t>知名私募/牛散</t>
   </si>
@@ -853,12 +853,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.05"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -898,13 +904,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="7" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.05"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1244,7 +1250,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1268,16 +1274,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1286,188 +1292,201 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="10" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="17" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="17" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="17" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="17" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1808,154 +1827,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="38"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="38"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="38"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="38"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="38"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="38"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="38" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1970,8 +1989,8 @@
   <sheetPr/>
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -1993,37 +2012,37 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="1" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1" spans="1:16">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
@@ -2066,7 +2085,7 @@
       <c r="O2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="1"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" ht="41" customHeight="1" spans="1:16">
       <c r="A3" s="9" t="s">
@@ -2351,81 +2370,81 @@
       <c r="P10" s="10"/>
     </row>
     <row r="11" ht="22.5" customHeight="1" spans="1:16">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="13">
         <v>2.9</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="13">
         <v>-2.5072</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="13">
         <v>8.1393</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="13">
         <v>4.522</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="22">
+      <c r="K11" s="25"/>
+      <c r="L11" s="26">
         <v>46059</v>
       </c>
-      <c r="M11" s="11" t="str">
+      <c r="M11" s="13" t="str">
         <f ca="1">DATEDIF(TODAY(),L11,"y")&amp;"年"&amp;DATEDIF(TODAY(),L11,"ym")&amp;"月"</f>
         <v>1年6月</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="N11" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="O11" s="21"/>
+      <c r="O11" s="25"/>
       <c r="P11" s="10">
         <f>SUM(B12:O12)</f>
         <v>2</v>
       </c>
     </row>
     <row r="12" ht="38" customHeight="1" spans="1:16">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11">
-        <v>1</v>
-      </c>
-      <c r="C12" s="11">
-        <v>0</v>
-      </c>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-      <c r="E12" s="11">
-        <v>1</v>
-      </c>
-      <c r="F12" s="11">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
         <v>2</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="23">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="27">
         <v>-1</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11">
+      <c r="J12" s="27"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13">
         <v>-1</v>
       </c>
-      <c r="O12" s="23"/>
+      <c r="O12" s="27"/>
       <c r="P12" s="10"/>
     </row>
     <row r="13" ht="22.5" customHeight="1" spans="1:16">
@@ -2480,12 +2499,12 @@
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="24"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
-      <c r="N14" s="25"/>
+      <c r="N14" s="28"/>
       <c r="O14" s="24"/>
       <c r="P14" s="10"/>
     </row>
@@ -2634,12 +2653,14 @@
       <c r="C19" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="11" t="s">
         <v>97</v>
       </c>
       <c r="F19" s="11">
-        <v>3.9</v>
+        <v>2.8</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>60</v>
@@ -2677,13 +2698,13 @@
         <v>0</v>
       </c>
       <c r="D20" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="11">
         <v>1</v>
       </c>
       <c r="F20" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -2963,13 +2984,13 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
-      <c r="K28" s="26">
+      <c r="K28" s="29">
         <v>-1</v>
       </c>
       <c r="L28" s="10"/>
       <c r="M28" s="12"/>
       <c r="N28" s="19"/>
-      <c r="O28" s="26"/>
+      <c r="O28" s="29"/>
       <c r="P28" s="10"/>
     </row>
     <row r="29" ht="36" customHeight="1" spans="1:16">
@@ -3002,7 +3023,7 @@
         <v>1.775</v>
       </c>
       <c r="K29" s="19"/>
-      <c r="L29" s="27">
+      <c r="L29" s="30">
         <v>46395</v>
       </c>
       <c r="M29" s="10" t="str">
@@ -3035,11 +3056,11 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
-      <c r="K30" s="26"/>
+      <c r="K30" s="29"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="19"/>
-      <c r="O30" s="26"/>
+      <c r="O30" s="29"/>
       <c r="P30" s="10"/>
     </row>
     <row r="31" ht="36" customHeight="1" spans="1:16">
@@ -3074,7 +3095,7 @@
         <v>5.237</v>
       </c>
       <c r="K31" s="19"/>
-      <c r="L31" s="27">
+      <c r="L31" s="30">
         <v>46427</v>
       </c>
       <c r="M31" s="10" t="str">
@@ -3109,11 +3130,11 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
-      <c r="K32" s="26"/>
+      <c r="K32" s="29"/>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="19"/>
-      <c r="O32" s="26"/>
+      <c r="O32" s="29"/>
       <c r="P32" s="10"/>
     </row>
     <row r="33" ht="36" customHeight="1" spans="1:16">
@@ -3170,11 +3191,11 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
-      <c r="K34" s="26"/>
+      <c r="K34" s="29"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="19"/>
-      <c r="O34" s="26"/>
+      <c r="O34" s="29"/>
       <c r="P34" s="10"/>
     </row>
     <row r="35" ht="36" customHeight="1" spans="1:16">
@@ -3231,11 +3252,11 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
-      <c r="K36" s="26"/>
+      <c r="K36" s="29"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="19"/>
-      <c r="O36" s="26"/>
+      <c r="O36" s="29"/>
       <c r="P36" s="10"/>
     </row>
     <row r="37" ht="36" customHeight="1" spans="1:16">
@@ -3514,11 +3535,11 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
-      <c r="K44" s="26"/>
+      <c r="K44" s="29"/>
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="19"/>
-      <c r="O44" s="26"/>
+      <c r="O44" s="29"/>
       <c r="P44" s="10"/>
     </row>
     <row r="45" ht="36" hidden="1" customHeight="1" spans="1:16">
@@ -3571,11 +3592,11 @@
       <c r="H46" s="10"/>
       <c r="I46" s="19"/>
       <c r="J46" s="19"/>
-      <c r="K46" s="26"/>
+      <c r="K46" s="29"/>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="N46" s="19"/>
-      <c r="O46" s="26"/>
+      <c r="O46" s="29"/>
       <c r="P46" s="10"/>
     </row>
     <row r="47" ht="36" customHeight="1" spans="1:16">
@@ -3630,7 +3651,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="19"/>
       <c r="J48" s="19"/>
-      <c r="K48" s="26"/>
+      <c r="K48" s="29"/>
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
       <c r="N48" s="19"/>
@@ -3663,10 +3684,10 @@
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
       <c r="K49" s="19"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
-      <c r="N49" s="28"/>
-      <c r="O49" s="29"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="32"/>
       <c r="P49" s="10">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -3694,10 +3715,10 @@
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
       <c r="K50" s="19"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="28"/>
-      <c r="O50" s="29"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="32"/>
       <c r="P50" s="10"/>
     </row>
     <row r="51" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -3806,15 +3827,15 @@
         <v>2.117</v>
       </c>
       <c r="K53" s="19"/>
-      <c r="L53" s="28" t="s">
+      <c r="L53" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="M53" s="28" t="str">
+      <c r="M53" s="31" t="str">
         <f ca="1">DATEDIF(TODAY(),L53,"y")&amp;"年"&amp;DATEDIF(TODAY(),L53,"ym")&amp;"月"</f>
         <v>3年11月</v>
       </c>
-      <c r="N53" s="28"/>
-      <c r="O53" s="29"/>
+      <c r="N53" s="31"/>
+      <c r="O53" s="32"/>
       <c r="P53" s="10">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -3842,10 +3863,10 @@
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
       <c r="K54" s="19"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="28"/>
-      <c r="N54" s="28"/>
-      <c r="O54" s="29"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
+      <c r="N54" s="31"/>
+      <c r="O54" s="32"/>
       <c r="P54" s="10"/>
     </row>
     <row r="55" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -3868,10 +3889,10 @@
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
       <c r="K55" s="19"/>
-      <c r="L55" s="28"/>
-      <c r="M55" s="28"/>
-      <c r="N55" s="28"/>
-      <c r="O55" s="29"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="32"/>
       <c r="P55" s="10">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -3895,10 +3916,10 @@
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
       <c r="K56" s="19"/>
-      <c r="L56" s="28"/>
-      <c r="M56" s="28"/>
-      <c r="N56" s="28"/>
-      <c r="O56" s="29"/>
+      <c r="L56" s="31"/>
+      <c r="M56" s="31"/>
+      <c r="N56" s="31"/>
+      <c r="O56" s="32"/>
       <c r="P56" s="10"/>
     </row>
     <row r="57" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -3923,10 +3944,10 @@
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="19"/>
-      <c r="L57" s="28"/>
-      <c r="M57" s="28"/>
-      <c r="N57" s="28"/>
-      <c r="O57" s="29"/>
+      <c r="L57" s="31"/>
+      <c r="M57" s="31"/>
+      <c r="N57" s="31"/>
+      <c r="O57" s="32"/>
       <c r="P57" s="10">
         <f t="shared" ref="P57:P61" si="4">SUM(B58:O58)</f>
         <v>4</v>
@@ -3952,10 +3973,10 @@
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
       <c r="K58" s="19"/>
-      <c r="L58" s="28"/>
-      <c r="M58" s="28"/>
-      <c r="N58" s="28"/>
-      <c r="O58" s="29"/>
+      <c r="L58" s="31"/>
+      <c r="M58" s="31"/>
+      <c r="N58" s="31"/>
+      <c r="O58" s="32"/>
       <c r="P58" s="10"/>
     </row>
     <row r="59" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -3982,10 +4003,10 @@
       <c r="I59" s="10"/>
       <c r="J59" s="10"/>
       <c r="K59" s="19"/>
-      <c r="L59" s="28"/>
-      <c r="M59" s="28"/>
-      <c r="N59" s="28"/>
-      <c r="O59" s="29"/>
+      <c r="L59" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="32"/>
       <c r="P59" s="10">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -4013,10 +4034,10 @@
       <c r="I60" s="10"/>
       <c r="J60" s="10"/>
       <c r="K60" s="19"/>
-      <c r="L60" s="28"/>
-      <c r="M60" s="28"/>
-      <c r="N60" s="28"/>
-      <c r="O60" s="29"/>
+      <c r="L60" s="31"/>
+      <c r="M60" s="31"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="32"/>
       <c r="P60" s="10"/>
     </row>
     <row r="61" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4043,10 +4064,10 @@
       <c r="I61" s="10"/>
       <c r="J61" s="10"/>
       <c r="K61" s="19"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="28"/>
-      <c r="N61" s="28"/>
-      <c r="O61" s="29"/>
+      <c r="L61" s="31"/>
+      <c r="M61" s="31"/>
+      <c r="N61" s="31"/>
+      <c r="O61" s="32"/>
       <c r="P61" s="10">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -4074,85 +4095,85 @@
       <c r="I62" s="10"/>
       <c r="J62" s="10"/>
       <c r="K62" s="19"/>
-      <c r="L62" s="28"/>
-      <c r="M62" s="28"/>
-      <c r="N62" s="28"/>
-      <c r="O62" s="29"/>
+      <c r="L62" s="31"/>
+      <c r="M62" s="31"/>
+      <c r="N62" s="31"/>
+      <c r="O62" s="32"/>
       <c r="P62" s="10"/>
     </row>
-    <row r="63" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A63" s="11" t="s">
+    <row r="63" s="1" customFormat="1" ht="36" customHeight="1" spans="1:16">
+      <c r="A63" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E63" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="F63" s="11">
+      <c r="F63" s="14">
         <v>3.4</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="G63" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H63" s="11">
+      <c r="H63" s="14">
         <v>-11.827</v>
       </c>
-      <c r="I63" s="11">
+      <c r="I63" s="14">
         <v>72.5556</v>
       </c>
-      <c r="J63" s="11">
+      <c r="J63" s="14">
         <v>26.508</v>
       </c>
-      <c r="K63" s="21"/>
-      <c r="L63" s="22">
+      <c r="K63" s="33"/>
+      <c r="L63" s="34">
         <v>46819</v>
       </c>
-      <c r="M63" s="11" t="str">
+      <c r="M63" s="14" t="str">
         <f ca="1">DATEDIF(TODAY(),L63,"y")&amp;"年"&amp;DATEDIF(TODAY(),L63,"ym")&amp;"月"</f>
         <v>3年7月</v>
       </c>
-      <c r="N63" s="11"/>
-      <c r="O63" s="21"/>
-      <c r="P63" s="10">
+      <c r="N63" s="14"/>
+      <c r="O63" s="33"/>
+      <c r="P63" s="14">
         <f>SUM(B64:O64)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="64" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11">
-        <v>1</v>
-      </c>
-      <c r="C64" s="11">
-        <v>0</v>
-      </c>
-      <c r="D64" s="11">
-        <v>1</v>
-      </c>
-      <c r="E64" s="11">
-        <v>1</v>
-      </c>
-      <c r="F64" s="11">
+    <row r="64" s="1" customFormat="1" ht="36" customHeight="1" spans="1:16">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14">
+        <v>1</v>
+      </c>
+      <c r="C64" s="14">
+        <v>0</v>
+      </c>
+      <c r="D64" s="14">
+        <v>1</v>
+      </c>
+      <c r="E64" s="14">
+        <v>1</v>
+      </c>
+      <c r="F64" s="14">
         <v>3</v>
       </c>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="21"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-      <c r="N64" s="11"/>
-      <c r="O64" s="21"/>
-      <c r="P64" s="10"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="14"/>
     </row>
     <row r="65" customFormat="1" ht="36" customHeight="1" spans="1:16">
       <c r="A65" s="10" t="s">
@@ -4176,10 +4197,10 @@
       <c r="I65" s="10"/>
       <c r="J65" s="10"/>
       <c r="K65" s="19"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="28"/>
-      <c r="N65" s="28"/>
-      <c r="O65" s="29"/>
+      <c r="L65" s="31"/>
+      <c r="M65" s="31"/>
+      <c r="N65" s="31"/>
+      <c r="O65" s="32"/>
       <c r="P65" s="10">
         <f>SUM(B66:O66)</f>
         <v>4</v>
@@ -4203,10 +4224,10 @@
       <c r="I66" s="10"/>
       <c r="J66" s="10"/>
       <c r="K66" s="19"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="28"/>
-      <c r="N66" s="28"/>
-      <c r="O66" s="29"/>
+      <c r="L66" s="31"/>
+      <c r="M66" s="31"/>
+      <c r="N66" s="31"/>
+      <c r="O66" s="32"/>
       <c r="P66" s="10"/>
     </row>
     <row r="67" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4299,15 +4320,15 @@
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
       <c r="K69" s="19"/>
-      <c r="L69" s="30">
+      <c r="L69" s="35">
         <v>46485</v>
       </c>
-      <c r="M69" s="28" t="str">
+      <c r="M69" s="31" t="str">
         <f ca="1">DATEDIF(TODAY(),L69,"y")&amp;"年"&amp;DATEDIF(TODAY(),L69,"ym")&amp;"月"</f>
         <v>2年8月</v>
       </c>
-      <c r="N69" s="28"/>
-      <c r="O69" s="29"/>
+      <c r="N69" s="31"/>
+      <c r="O69" s="32"/>
       <c r="P69" s="10">
         <f t="shared" ref="P69:P73" si="5">SUM(B70:O70)</f>
         <v>4</v>
@@ -4331,10 +4352,10 @@
       <c r="I70" s="10"/>
       <c r="J70" s="10"/>
       <c r="K70" s="19"/>
-      <c r="L70" s="28"/>
-      <c r="M70" s="28"/>
-      <c r="N70" s="28"/>
-      <c r="O70" s="29"/>
+      <c r="L70" s="31"/>
+      <c r="M70" s="31"/>
+      <c r="N70" s="31"/>
+      <c r="O70" s="32"/>
       <c r="P70" s="10"/>
     </row>
     <row r="71" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4357,10 +4378,10 @@
       <c r="I71" s="10"/>
       <c r="J71" s="10"/>
       <c r="K71" s="19"/>
-      <c r="L71" s="28"/>
-      <c r="M71" s="28"/>
-      <c r="N71" s="28"/>
-      <c r="O71" s="29"/>
+      <c r="L71" s="31"/>
+      <c r="M71" s="31"/>
+      <c r="N71" s="31"/>
+      <c r="O71" s="32"/>
       <c r="P71" s="10">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -4384,10 +4405,10 @@
       <c r="I72" s="10"/>
       <c r="J72" s="10"/>
       <c r="K72" s="19"/>
-      <c r="L72" s="28"/>
-      <c r="M72" s="28"/>
-      <c r="N72" s="28"/>
-      <c r="O72" s="29"/>
+      <c r="L72" s="31"/>
+      <c r="M72" s="31"/>
+      <c r="N72" s="31"/>
+      <c r="O72" s="32"/>
       <c r="P72" s="10"/>
     </row>
     <row r="73" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4469,7 +4490,9 @@
         <v>200</v>
       </c>
       <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="E75" s="11" t="s">
+        <v>193</v>
+      </c>
       <c r="F75" s="11">
         <v>2.5</v>
       </c>
@@ -4499,7 +4522,7 @@
       <c r="O75" s="21"/>
       <c r="P75" s="10">
         <f t="shared" ref="P75:P79" si="7">SUM(B76:O76)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4509,7 +4532,9 @@
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="E76" s="11">
+        <v>1</v>
+      </c>
       <c r="F76" s="11">
         <v>2</v>
       </c>
@@ -4527,75 +4552,75 @@
       <c r="P76" s="10"/>
     </row>
     <row r="77" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11" t="s">
+      <c r="B77" s="13"/>
+      <c r="C77" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E77" s="11" t="s">
+      <c r="E77" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="F77" s="11">
+      <c r="F77" s="13">
         <v>2.5</v>
       </c>
-      <c r="G77" s="11" t="s">
+      <c r="G77" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H77" s="11">
+      <c r="H77" s="13">
         <v>8.4979</v>
       </c>
-      <c r="I77" s="11">
+      <c r="I77" s="13">
         <v>205.2484</v>
       </c>
-      <c r="J77" s="11">
+      <c r="J77" s="13">
         <v>3.24</v>
       </c>
-      <c r="K77" s="21" t="s">
+      <c r="K77" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="L77" s="22">
+      <c r="L77" s="26">
         <v>46371</v>
       </c>
-      <c r="M77" s="21" t="str">
+      <c r="M77" s="25" t="str">
         <f ca="1" t="shared" si="6"/>
         <v>2年5月</v>
       </c>
-      <c r="N77" s="21"/>
-      <c r="O77" s="21"/>
+      <c r="N77" s="25"/>
+      <c r="O77" s="25"/>
       <c r="P77" s="10">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
     <row r="78" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11">
-        <v>1</v>
-      </c>
-      <c r="E78" s="11">
-        <v>1</v>
-      </c>
-      <c r="F78" s="11">
+      <c r="A78" s="13"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13">
+        <v>1</v>
+      </c>
+      <c r="E78" s="13">
+        <v>1</v>
+      </c>
+      <c r="F78" s="13">
         <v>2</v>
       </c>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
-      <c r="K78" s="23">
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="27">
         <v>-1</v>
       </c>
-      <c r="L78" s="22"/>
-      <c r="M78" s="21"/>
-      <c r="N78" s="21"/>
-      <c r="O78" s="21"/>
+      <c r="L78" s="26"/>
+      <c r="M78" s="25"/>
+      <c r="N78" s="25"/>
+      <c r="O78" s="25"/>
       <c r="P78" s="10"/>
     </row>
     <row r="79" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4627,9 +4652,7 @@
       <c r="J79" s="11">
         <v>11.45</v>
       </c>
-      <c r="K79" s="21" t="s">
-        <v>61</v>
-      </c>
+      <c r="K79" s="21"/>
       <c r="L79" s="22">
         <v>46017</v>
       </c>

</xml_diff>

<commit_message>
1.update kgooglist add shanshi bond
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="7140"/>
+    <workbookView windowWidth="18350" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="213">
   <si>
     <t>知名私募/牛散</t>
   </si>
@@ -662,6 +662,12 @@
   </si>
   <si>
     <t>光模块</t>
+  </si>
+  <si>
+    <t>山石转债</t>
+  </si>
+  <si>
+    <t>信息安全</t>
   </si>
 </sst>
 </file>
@@ -1844,7 +1850,7 @@
   <sheetPr/>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -2016,10 +2022,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -2216,7 +2222,7 @@
       </c>
       <c r="M5" s="12" t="str">
         <f ca="1">DATEDIF(TODAY(),L5,"y")&amp;"年"&amp;DATEDIF(TODAY(),L5,"ym")&amp;"月"</f>
-        <v>1年0月</v>
+        <v>0年11月</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="21" t="s">
@@ -2296,7 +2302,7 @@
       </c>
       <c r="M7" s="13" t="str">
         <f ca="1">DATEDIF(TODAY(),L7,"y")&amp;"年"&amp;DATEDIF(TODAY(),L7,"ym")&amp;"月"</f>
-        <v>1年1月</v>
+        <v>0年11月</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>70</v>
@@ -2433,7 +2439,7 @@
       </c>
       <c r="M11" s="15" t="str">
         <f ca="1">DATEDIF(TODAY(),L11,"y")&amp;"年"&amp;DATEDIF(TODAY(),L11,"ym")&amp;"月"</f>
-        <v>1年4月</v>
+        <v>1年3月</v>
       </c>
       <c r="N11" s="15" t="s">
         <v>80</v>
@@ -2574,7 +2580,7 @@
       </c>
       <c r="M15" s="13" t="str">
         <f ca="1">DATEDIF(TODAY(),L15,"y")&amp;"年"&amp;DATEDIF(TODAY(),L15,"ym")&amp;"月"</f>
-        <v>1年3月</v>
+        <v>1年1月</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="23"/>
@@ -2709,7 +2715,7 @@
       </c>
       <c r="M19" s="13" t="str">
         <f ca="1" t="shared" ref="M19:M23" si="0">DATEDIF(TODAY(),L19,"y")&amp;"年"&amp;DATEDIF(TODAY(),L19,"ym")&amp;"月"</f>
-        <v>1年10月</v>
+        <v>1年8月</v>
       </c>
       <c r="N19" s="13"/>
       <c r="O19" s="23"/>
@@ -2785,7 +2791,7 @@
       </c>
       <c r="M21" s="13" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>2年3月</v>
+        <v>2年2月</v>
       </c>
       <c r="N21" s="13"/>
       <c r="O21" s="23"/>
@@ -2861,7 +2867,7 @@
       </c>
       <c r="M23" s="13" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>2年2月</v>
+        <v>2年1月</v>
       </c>
       <c r="N23" s="13"/>
       <c r="O23" s="23"/>
@@ -3058,8 +3064,8 @@
         <v>46395</v>
       </c>
       <c r="M29" s="13" t="str">
-        <f ca="1">DATEDIF(TODAY(),L29,"y")&amp;"年"&amp;DATEDIF(TODAY(),L29,"ym")&amp;"月"</f>
-        <v>2年3月</v>
+        <f ca="1" t="shared" ref="M29:M33" si="1">DATEDIF(TODAY(),L29,"y")&amp;"年"&amp;DATEDIF(TODAY(),L29,"ym")&amp;"月"</f>
+        <v>2年2月</v>
       </c>
       <c r="N29" s="13"/>
       <c r="O29" s="23"/>
@@ -3130,8 +3136,8 @@
         <v>46427</v>
       </c>
       <c r="M31" s="12" t="str">
-        <f ca="1">DATEDIF(TODAY(),L31,"y")&amp;"年"&amp;DATEDIF(TODAY(),L31,"ym")&amp;"月"</f>
-        <v>2年4月</v>
+        <f ca="1" t="shared" si="1"/>
+        <v>2年3月</v>
       </c>
       <c r="N31" s="12"/>
       <c r="O31" s="21"/>
@@ -3168,66 +3174,79 @@
       <c r="O32" s="31"/>
       <c r="P32" s="12"/>
     </row>
-    <row r="33" ht="36" customHeight="1" spans="1:16">
-      <c r="A33" s="12" t="s">
+    <row r="33" s="1" customFormat="1" ht="36" customHeight="1" spans="1:16">
+      <c r="A33" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="13">
         <v>3.8</v>
       </c>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="12">
+      <c r="G33" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="13">
+        <v>-5.1888</v>
+      </c>
+      <c r="I33" s="13">
+        <v>77.2377</v>
+      </c>
+      <c r="J33" s="13">
+        <v>7.395</v>
+      </c>
+      <c r="K33" s="23"/>
+      <c r="L33" s="24">
+        <v>46269</v>
+      </c>
+      <c r="M33" s="13" t="str">
+        <f ca="1" t="shared" si="1"/>
+        <v>1年10月</v>
+      </c>
+      <c r="N33" s="13"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="13">
         <f>SUM(B34:O34)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="34" ht="38" customHeight="1" spans="1:16">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12">
-        <v>0</v>
-      </c>
-      <c r="C34" s="12">
-        <v>0</v>
-      </c>
-      <c r="D34" s="12">
-        <v>1</v>
-      </c>
-      <c r="E34" s="12">
-        <v>1</v>
-      </c>
-      <c r="F34" s="12">
+    <row r="34" s="1" customFormat="1" ht="38" customHeight="1" spans="1:16">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13">
+        <v>0</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0</v>
+      </c>
+      <c r="D34" s="13">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13">
+        <v>1</v>
+      </c>
+      <c r="F34" s="13">
         <v>3</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="12"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="13"/>
     </row>
     <row r="35" ht="36" customHeight="1" spans="1:16">
       <c r="A35" s="12" t="s">
@@ -3326,8 +3345,8 @@
         <v>46223</v>
       </c>
       <c r="M37" s="13" t="str">
-        <f ca="1" t="shared" ref="M37:M41" si="1">DATEDIF(TODAY(),L37,"y")&amp;"年"&amp;DATEDIF(TODAY(),L37,"ym")&amp;"月"</f>
-        <v>1年9月</v>
+        <f ca="1" t="shared" ref="M37:M41" si="2">DATEDIF(TODAY(),L37,"y")&amp;"年"&amp;DATEDIF(TODAY(),L37,"ym")&amp;"月"</f>
+        <v>1年8月</v>
       </c>
       <c r="N37" s="13"/>
       <c r="O37" s="23"/>
@@ -3400,8 +3419,8 @@
         <v>46640</v>
       </c>
       <c r="M39" s="13" t="str">
-        <f ca="1" t="shared" si="1"/>
-        <v>2年11月</v>
+        <f ca="1" t="shared" si="2"/>
+        <v>2年10月</v>
       </c>
       <c r="N39" s="13"/>
       <c r="O39" s="23"/>
@@ -3474,8 +3493,8 @@
         <v>46129</v>
       </c>
       <c r="M41" s="13" t="str">
-        <f ca="1" t="shared" si="1"/>
-        <v>1年6月</v>
+        <f ca="1" t="shared" si="2"/>
+        <v>1年5月</v>
       </c>
       <c r="N41" s="13" t="s">
         <v>70</v>
@@ -3600,7 +3619,7 @@
       <c r="N45" s="12"/>
       <c r="O45" s="21"/>
       <c r="P45" s="12">
-        <f t="shared" ref="P45:P49" si="2">SUM(B46:O46)</f>
+        <f t="shared" ref="P45:P49" si="3">SUM(B46:O46)</f>
         <v>4</v>
       </c>
     </row>
@@ -3659,7 +3678,7 @@
         <v>62</v>
       </c>
       <c r="P47" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -3720,7 +3739,7 @@
       <c r="N49" s="33"/>
       <c r="O49" s="34"/>
       <c r="P49" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -3789,12 +3808,12 @@
       </c>
       <c r="M51" s="16" t="str">
         <f ca="1">DATEDIF(TODAY(),L51,"y")&amp;"年"&amp;DATEDIF(TODAY(),L51,"ym")&amp;"月"</f>
-        <v>2年3月</v>
+        <v>2年2月</v>
       </c>
       <c r="N51" s="16"/>
       <c r="O51" s="35"/>
       <c r="P51" s="16">
-        <f t="shared" ref="P51:P55" si="3">SUM(B52:O52)</f>
+        <f t="shared" ref="P51:P55" si="4">SUM(B52:O52)</f>
         <v>5</v>
       </c>
     </row>
@@ -3863,12 +3882,12 @@
       </c>
       <c r="M53" s="33" t="str">
         <f ca="1">DATEDIF(TODAY(),L53,"y")&amp;"年"&amp;DATEDIF(TODAY(),L53,"ym")&amp;"月"</f>
-        <v>3年9月</v>
+        <v>3年8月</v>
       </c>
       <c r="N53" s="33"/>
       <c r="O53" s="34"/>
       <c r="P53" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -3925,7 +3944,7 @@
       <c r="N55" s="33"/>
       <c r="O55" s="34"/>
       <c r="P55" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -3980,7 +3999,7 @@
       <c r="N57" s="33"/>
       <c r="O57" s="34"/>
       <c r="P57" s="12">
-        <f t="shared" ref="P57:P61" si="4">SUM(B58:O58)</f>
+        <f t="shared" ref="P57:P61" si="5">SUM(B58:O58)</f>
         <v>4</v>
       </c>
     </row>
@@ -4039,7 +4058,7 @@
       <c r="N59" s="33"/>
       <c r="O59" s="34"/>
       <c r="P59" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -4100,7 +4119,7 @@
       <c r="N61" s="33"/>
       <c r="O61" s="34"/>
       <c r="P61" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -4171,7 +4190,7 @@
       </c>
       <c r="M63" s="13" t="str">
         <f ca="1">DATEDIF(TODAY(),L63,"y")&amp;"年"&amp;DATEDIF(TODAY(),L63,"ym")&amp;"月"</f>
-        <v>3年5月</v>
+        <v>3年4月</v>
       </c>
       <c r="N63" s="13"/>
       <c r="O63" s="23"/>
@@ -4243,7 +4262,7 @@
       </c>
       <c r="M65" s="37" t="str">
         <f ca="1">DATEDIF(TODAY(),L65,"y")&amp;"年"&amp;DATEDIF(TODAY(),L65,"ym")&amp;"月"</f>
-        <v>1年10月</v>
+        <v>1年9月</v>
       </c>
       <c r="N65" s="37"/>
       <c r="O65" s="38"/>
@@ -4313,7 +4332,7 @@
       </c>
       <c r="M67" s="37" t="str">
         <f ca="1">DATEDIF(TODAY(),L67,"y")&amp;"年"&amp;DATEDIF(TODAY(),L67,"ym")&amp;"月"</f>
-        <v>1年9月</v>
+        <v>1年8月</v>
       </c>
       <c r="N67" s="37"/>
       <c r="O67" s="38"/>
@@ -4371,12 +4390,12 @@
       </c>
       <c r="M69" s="33" t="str">
         <f ca="1">DATEDIF(TODAY(),L69,"y")&amp;"年"&amp;DATEDIF(TODAY(),L69,"ym")&amp;"月"</f>
-        <v>2年6月</v>
+        <v>2年5月</v>
       </c>
       <c r="N69" s="33"/>
       <c r="O69" s="34"/>
       <c r="P69" s="12">
-        <f t="shared" ref="P69:P73" si="5">SUM(B70:O70)</f>
+        <f t="shared" ref="P69:P73" si="6">SUM(B70:O70)</f>
         <v>4</v>
       </c>
     </row>
@@ -4429,7 +4448,7 @@
       <c r="N71" s="33"/>
       <c r="O71" s="34"/>
       <c r="P71" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -4491,13 +4510,13 @@
         <v>46955</v>
       </c>
       <c r="M73" s="23" t="str">
-        <f ca="1" t="shared" ref="M73:M77" si="6">DATEDIF(TODAY(),L73,"y")&amp;"年"&amp;DATEDIF(TODAY(),L73,"ym")&amp;"月"</f>
-        <v>3年10月</v>
+        <f ca="1" t="shared" ref="M73:M77" si="7">DATEDIF(TODAY(),L73,"y")&amp;"年"&amp;DATEDIF(TODAY(),L73,"ym")&amp;"月"</f>
+        <v>3年8月</v>
       </c>
       <c r="N73" s="23"/>
       <c r="O73" s="23"/>
       <c r="P73" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -4559,15 +4578,15 @@
         <v>46220</v>
       </c>
       <c r="M75" s="23" t="str">
-        <f ca="1" t="shared" si="6"/>
-        <v>1年9月</v>
+        <f ca="1" t="shared" si="7"/>
+        <v>1年8月</v>
       </c>
       <c r="N75" s="23" t="s">
         <v>70</v>
       </c>
       <c r="O75" s="23"/>
       <c r="P75" s="12">
-        <f t="shared" ref="P75:P79" si="7">SUM(B76:O76)</f>
+        <f t="shared" ref="P75:P79" si="8">SUM(B76:O76)</f>
         <v>5</v>
       </c>
     </row>
@@ -4633,13 +4652,13 @@
         <v>46371</v>
       </c>
       <c r="M77" s="27" t="str">
-        <f ca="1" t="shared" si="6"/>
-        <v>2年2月</v>
+        <f ca="1" t="shared" si="7"/>
+        <v>2年1月</v>
       </c>
       <c r="N77" s="27"/>
       <c r="O77" s="27"/>
       <c r="P77" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -4705,13 +4724,13 @@
         <v>46017</v>
       </c>
       <c r="M79" s="23" t="str">
-        <f ca="1">DATEDIF(TODAY(),L79,"y")&amp;"年"&amp;DATEDIF(TODAY(),L79,"ym")&amp;"月"</f>
-        <v>1年3月</v>
+        <f ca="1" t="shared" ref="M79:M83" si="9">DATEDIF(TODAY(),L79,"y")&amp;"年"&amp;DATEDIF(TODAY(),L79,"ym")&amp;"月"</f>
+        <v>1年1月</v>
       </c>
       <c r="N79" s="23"/>
       <c r="O79" s="23"/>
       <c r="P79" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -4773,8 +4792,8 @@
         <v>46371</v>
       </c>
       <c r="M81" s="23" t="str">
-        <f ca="1">DATEDIF(TODAY(),L81,"y")&amp;"年"&amp;DATEDIF(TODAY(),L81,"ym")&amp;"月"</f>
-        <v>2年2月</v>
+        <f ca="1" t="shared" si="9"/>
+        <v>2年1月</v>
       </c>
       <c r="N81" s="23" t="s">
         <v>70</v>
@@ -4811,8 +4830,76 @@
       <c r="O82" s="23"/>
       <c r="P82" s="12"/>
     </row>
+    <row r="83" customFormat="1" ht="36" customHeight="1" spans="1:16">
+      <c r="A83" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F83" s="13">
+        <v>3.4</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H83" s="13">
+        <v>-17.3438</v>
+      </c>
+      <c r="I83" s="13">
+        <v>34.7786</v>
+      </c>
+      <c r="J83" s="13">
+        <v>5.548</v>
+      </c>
+      <c r="K83" s="23"/>
+      <c r="L83" s="24">
+        <v>46834</v>
+      </c>
+      <c r="M83" s="23" t="str">
+        <f ca="1" t="shared" si="9"/>
+        <v>3年4月</v>
+      </c>
+      <c r="N83" s="23"/>
+      <c r="O83" s="23"/>
+      <c r="P83" s="12">
+        <f>SUM(B84:O84)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" customFormat="1" ht="36" customHeight="1" spans="1:16">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13">
+        <v>1</v>
+      </c>
+      <c r="E84" s="13">
+        <v>1</v>
+      </c>
+      <c r="F84" s="13">
+        <v>3</v>
+      </c>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="25"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="23"/>
+      <c r="N84" s="25"/>
+      <c r="O84" s="23"/>
+      <c r="P84" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="86">
+  <mergeCells count="88">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -4858,6 +4945,7 @@
     <mergeCell ref="A77:A78"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A84"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="P5:P6"/>
@@ -4899,6 +4987,7 @@
     <mergeCell ref="P77:P78"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="P81:P82"/>
+    <mergeCell ref="P83:P84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1.golden the bonded which maked money
</commit_message>
<xml_diff>
--- a/kgoodlist.xlsx
+++ b/kgoodlist.xlsx
@@ -877,18 +877,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF96EEFB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -922,6 +916,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF96EEFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.05"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -929,6 +929,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1274,7 +1280,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1298,16 +1304,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1316,190 +1322,232 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="11" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="10" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="10" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1514,14 +1562,14 @@
     <xf numFmtId="14" fontId="4" fillId="8" borderId="6" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="17" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="17" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="17" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="17" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1862,154 +1910,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="57"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="57"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="57"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="58" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="57"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="57"/>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="57"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="43"/>
+      <c r="C9" s="57"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="43"/>
+      <c r="C10" s="57"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="57"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="56" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="57" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="57" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2022,10 +2070,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:NX84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -2143,14 +2191,14 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="21" t="s">
         <v>55</v>
       </c>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="11">
+      <c r="O3" s="21"/>
+      <c r="P3" s="12">
         <f>SUM(B4:O4)</f>
         <v>2</v>
       </c>
@@ -2176,14 +2224,14 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="18">
+      <c r="K4" s="22">
         <v>-2</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="11"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="12"/>
     </row>
     <row r="5" ht="36" customHeight="1" spans="1:16">
       <c r="A5" s="12" t="s">
@@ -2208,24 +2256,24 @@
       <c r="H5" s="12">
         <v>1.7207</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="23">
         <v>185.9515</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="24">
         <v>4.816</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="26">
         <v>45944</v>
       </c>
       <c r="M5" s="12" t="str">
         <f ca="1">DATEDIF(TODAY(),L5,"y")&amp;"年"&amp;DATEDIF(TODAY(),L5,"ym")&amp;"月"</f>
-        <v>0年11月</v>
+        <v>0年9月</v>
       </c>
       <c r="N5" s="12"/>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="25" t="s">
         <v>62</v>
       </c>
       <c r="P5" s="12">
@@ -2254,13 +2302,13 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="25" t="s">
         <v>63</v>
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
-      <c r="O6" s="21">
+      <c r="O6" s="25">
         <v>-1</v>
       </c>
       <c r="P6" s="12"/>
@@ -2296,18 +2344,18 @@
       <c r="J7" s="13">
         <v>2.37</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24">
+      <c r="K7" s="27"/>
+      <c r="L7" s="28">
         <v>45953</v>
       </c>
       <c r="M7" s="13" t="str">
         <f ca="1">DATEDIF(TODAY(),L7,"y")&amp;"年"&amp;DATEDIF(TODAY(),L7,"ym")&amp;"月"</f>
-        <v>0年11月</v>
+        <v>0年9月</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="O7" s="23"/>
+      <c r="O7" s="27"/>
       <c r="P7" s="12">
         <f>SUM(B8:O8)</f>
         <v>7</v>
@@ -2334,13 +2382,13 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="23"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13">
         <v>1</v>
       </c>
-      <c r="O8" s="25"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="12"/>
     </row>
     <row r="9" ht="22.5" customHeight="1" spans="1:16">
@@ -2366,11 +2414,11 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="26"/>
+      <c r="K9" s="30"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="26"/>
+      <c r="O9" s="30"/>
       <c r="P9" s="12">
         <f>SUM(B10:O10)</f>
         <v>5</v>
@@ -2397,11 +2445,11 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="26"/>
+      <c r="K10" s="30"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
-      <c r="O10" s="26"/>
+      <c r="O10" s="30"/>
       <c r="P10" s="12"/>
     </row>
     <row r="11" ht="22.5" customHeight="1" spans="1:16">
@@ -2433,18 +2481,18 @@
       <c r="J11" s="15">
         <v>4.522</v>
       </c>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28">
+      <c r="K11" s="31"/>
+      <c r="L11" s="32">
         <v>46059</v>
       </c>
       <c r="M11" s="15" t="str">
         <f ca="1">DATEDIF(TODAY(),L11,"y")&amp;"年"&amp;DATEDIF(TODAY(),L11,"ym")&amp;"月"</f>
-        <v>1年3月</v>
+        <v>1年1月</v>
       </c>
       <c r="N11" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="27"/>
+      <c r="O11" s="31"/>
       <c r="P11" s="12">
         <f>SUM(B12:O12)</f>
         <v>2</v>
@@ -2469,17 +2517,17 @@
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="29">
+      <c r="I12" s="33">
         <v>-1</v>
       </c>
-      <c r="J12" s="29"/>
-      <c r="K12" s="27"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="31"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
       <c r="N12" s="15">
         <v>-1</v>
       </c>
-      <c r="O12" s="29"/>
+      <c r="O12" s="33"/>
       <c r="P12" s="12"/>
     </row>
     <row r="13" ht="22.5" customHeight="1" spans="1:16">
@@ -2505,11 +2553,11 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="26"/>
+      <c r="K13" s="30"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
-      <c r="O13" s="26"/>
+      <c r="O13" s="30"/>
       <c r="P13" s="12">
         <f>SUM(B14:O14)</f>
         <v>6</v>
@@ -2534,87 +2582,87 @@
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="26"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="30"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="26"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="30"/>
       <c r="P14" s="12"/>
     </row>
     <row r="15" ht="22.5" customHeight="1" spans="1:16">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="16">
         <v>2.4</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="16">
         <v>6.1553</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="16">
         <v>30.6692</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="16">
         <v>28.303</v>
       </c>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24">
+      <c r="K15" s="35"/>
+      <c r="L15" s="36">
         <v>46018</v>
       </c>
-      <c r="M15" s="13" t="str">
+      <c r="M15" s="16" t="str">
         <f ca="1">DATEDIF(TODAY(),L15,"y")&amp;"年"&amp;DATEDIF(TODAY(),L15,"ym")&amp;"月"</f>
-        <v>1年1月</v>
-      </c>
-      <c r="N15" s="13"/>
-      <c r="O15" s="23"/>
+        <v>0年11月</v>
+      </c>
+      <c r="N15" s="16"/>
+      <c r="O15" s="35"/>
       <c r="P15" s="12">
         <f>SUM(B16:O16)</f>
         <v>4</v>
       </c>
     </row>
     <row r="16" ht="38" customHeight="1" spans="1:16">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16">
         <v>0</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="16">
         <v>0</v>
       </c>
-      <c r="D16" s="13">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13">
-        <v>1</v>
-      </c>
-      <c r="F16" s="13">
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="16">
         <v>2</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="25"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="37"/>
       <c r="P16" s="12"/>
     </row>
     <row r="17" ht="22.5" customHeight="1" spans="1:16">
@@ -2640,11 +2688,11 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
-      <c r="K17" s="21"/>
+      <c r="K17" s="25"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
-      <c r="O17" s="21"/>
+      <c r="O17" s="25"/>
       <c r="P17" s="12">
         <f>SUM(B18:O18)</f>
         <v>4</v>
@@ -2669,87 +2717,87 @@
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
       <c r="P18" s="12"/>
     </row>
     <row r="19" ht="22.5" customHeight="1" spans="1:16">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="16">
         <v>2.8</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="16">
         <v>-0.392</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="16">
         <v>23.9756</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="16">
         <v>10.093</v>
       </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24">
+      <c r="K19" s="35"/>
+      <c r="L19" s="36">
         <v>46225</v>
       </c>
-      <c r="M19" s="13" t="str">
+      <c r="M19" s="16" t="str">
         <f ca="1" t="shared" ref="M19:M23" si="0">DATEDIF(TODAY(),L19,"y")&amp;"年"&amp;DATEDIF(TODAY(),L19,"ym")&amp;"月"</f>
-        <v>1年8月</v>
-      </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="23"/>
+        <v>1年6月</v>
+      </c>
+      <c r="N19" s="16"/>
+      <c r="O19" s="35"/>
       <c r="P19" s="12">
         <f>SUM(B20:O20)</f>
         <v>4</v>
       </c>
     </row>
     <row r="20" ht="38" customHeight="1" spans="1:16">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16">
         <v>0</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="16">
         <v>0</v>
       </c>
-      <c r="D20" s="13">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13">
-        <v>1</v>
-      </c>
-      <c r="F20" s="13">
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16">
         <v>2</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
       <c r="P20" s="12"/>
     </row>
     <row r="21" ht="37" customHeight="1" spans="1:16">
@@ -2783,18 +2831,18 @@
       <c r="J21" s="13">
         <v>1.999</v>
       </c>
-      <c r="K21" s="23" t="s">
+      <c r="K21" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="28">
         <v>46406</v>
       </c>
       <c r="M21" s="13" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>2年2月</v>
+        <v>2年0月</v>
       </c>
       <c r="N21" s="13"/>
-      <c r="O21" s="23"/>
+      <c r="O21" s="27"/>
       <c r="P21" s="12">
         <f>SUM(B22:O22)</f>
         <v>8</v>
@@ -2819,13 +2867,13 @@
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
       <c r="P22" s="12"/>
     </row>
     <row r="23" ht="28" customHeight="1" spans="1:16">
@@ -2859,18 +2907,18 @@
       <c r="J23" s="13">
         <v>5.06</v>
       </c>
-      <c r="K23" s="23" t="s">
+      <c r="K23" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="L23" s="24">
+      <c r="L23" s="28">
         <v>46363</v>
       </c>
       <c r="M23" s="13" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>2年1月</v>
+        <v>1年11月</v>
       </c>
       <c r="N23" s="13"/>
-      <c r="O23" s="23"/>
+      <c r="O23" s="27"/>
       <c r="P23" s="12">
         <f>SUM(B24:O24)</f>
         <v>7</v>
@@ -2895,72 +2943,72 @@
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
       <c r="P24" s="12"/>
     </row>
     <row r="25" ht="36" customHeight="1" spans="1:16">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="16">
         <v>6.2</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="26"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="35"/>
       <c r="P25" s="12">
         <f>SUM(B26:O26)</f>
         <v>7</v>
       </c>
     </row>
     <row r="26" ht="38" customHeight="1" spans="1:16">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16">
         <v>0</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="16">
         <v>0</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="16">
         <v>0</v>
       </c>
-      <c r="E26" s="14">
-        <v>1</v>
-      </c>
-      <c r="F26" s="14">
+      <c r="E26" s="16">
+        <v>1</v>
+      </c>
+      <c r="F26" s="16">
         <v>6</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
       <c r="P26" s="12"/>
     </row>
     <row r="27" ht="36" customHeight="1" spans="1:16">
@@ -2986,13 +3034,13 @@
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
-      <c r="K27" s="21" t="s">
+      <c r="K27" s="25" t="s">
         <v>117</v>
       </c>
       <c r="L27" s="12"/>
       <c r="M27" s="14"/>
       <c r="N27" s="12"/>
-      <c r="O27" s="21"/>
+      <c r="O27" s="25"/>
       <c r="P27" s="12">
         <f>SUM(B28:O28)</f>
         <v>7</v>
@@ -3017,88 +3065,88 @@
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="31">
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="38">
         <v>-1</v>
       </c>
       <c r="L28" s="12"/>
       <c r="M28" s="14"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="31"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="38"/>
       <c r="P28" s="12"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="16">
         <v>5.06</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="16">
         <v>3.9695</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="16">
         <v>65.6913</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="16">
         <v>1.977</v>
       </c>
-      <c r="K29" s="23" t="s">
+      <c r="K29" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="L29" s="24">
+      <c r="L29" s="36">
         <v>46395</v>
       </c>
-      <c r="M29" s="13" t="str">
+      <c r="M29" s="16" t="str">
         <f ca="1" t="shared" ref="M29:M33" si="1">DATEDIF(TODAY(),L29,"y")&amp;"年"&amp;DATEDIF(TODAY(),L29,"ym")&amp;"月"</f>
-        <v>2年2月</v>
-      </c>
-      <c r="N29" s="13"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="13">
+        <v>2年0月</v>
+      </c>
+      <c r="N29" s="16"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="39">
         <f>SUM(B30:O30)</f>
         <v>7</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="38" customHeight="1" spans="1:16">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13">
-        <v>1</v>
-      </c>
-      <c r="C30" s="13">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16">
+        <v>1</v>
+      </c>
+      <c r="C30" s="16">
         <v>0</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13">
-        <v>1</v>
-      </c>
-      <c r="F30" s="13">
+      <c r="D30" s="16"/>
+      <c r="E30" s="16">
+        <v>1</v>
+      </c>
+      <c r="F30" s="16">
         <v>5</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="13"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="37"/>
+      <c r="P30" s="39"/>
     </row>
     <row r="31" ht="36" customHeight="1" spans="1:16">
       <c r="A31" s="12" t="s">
@@ -3131,16 +3179,16 @@
       <c r="J31" s="12">
         <v>5.237</v>
       </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="32">
+      <c r="K31" s="25"/>
+      <c r="L31" s="40">
         <v>46427</v>
       </c>
       <c r="M31" s="12" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>2年3月</v>
+        <v>2年1月</v>
       </c>
       <c r="N31" s="12"/>
-      <c r="O31" s="21"/>
+      <c r="O31" s="25"/>
       <c r="P31" s="12">
         <f>SUM(B32:O32)</f>
         <v>6</v>
@@ -3165,13 +3213,13 @@
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="31"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="38"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="31"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="38"/>
       <c r="P32" s="12"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -3205,17 +3253,17 @@
       <c r="J33" s="13">
         <v>7.395</v>
       </c>
-      <c r="K33" s="23"/>
-      <c r="L33" s="24">
+      <c r="K33" s="27"/>
+      <c r="L33" s="28">
         <v>46269</v>
       </c>
       <c r="M33" s="13" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>1年10月</v>
+        <v>1年8月</v>
       </c>
       <c r="N33" s="13"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="13">
+      <c r="O33" s="27"/>
+      <c r="P33" s="39">
         <f>SUM(B34:O34)</f>
         <v>5</v>
       </c>
@@ -3239,74 +3287,74 @@
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="25"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="29"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="13"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="39"/>
     </row>
     <row r="35" ht="36" customHeight="1" spans="1:16">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="17">
         <v>3.6</v>
       </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="21"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="41"/>
       <c r="P35" s="12">
         <f>SUM(B36:O36)</f>
         <v>6</v>
       </c>
     </row>
     <row r="36" ht="38" customHeight="1" spans="1:16">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12">
-        <v>1</v>
-      </c>
-      <c r="C36" s="12">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17">
+        <v>1</v>
+      </c>
+      <c r="C36" s="17">
         <v>0</v>
       </c>
-      <c r="D36" s="12">
-        <v>1</v>
-      </c>
-      <c r="E36" s="12">
-        <v>1</v>
-      </c>
-      <c r="F36" s="12">
+      <c r="D36" s="17">
+        <v>1</v>
+      </c>
+      <c r="E36" s="17">
+        <v>1</v>
+      </c>
+      <c r="F36" s="17">
         <v>3</v>
       </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="31"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="42"/>
       <c r="P36" s="12"/>
     </row>
     <row r="37" ht="36" customHeight="1" spans="1:16">
@@ -3338,18 +3386,18 @@
       <c r="J37" s="13">
         <v>5.3888</v>
       </c>
-      <c r="K37" s="23" t="s">
+      <c r="K37" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="L37" s="24">
+      <c r="L37" s="28">
         <v>46223</v>
       </c>
       <c r="M37" s="13" t="str">
         <f ca="1" t="shared" ref="M37:M41" si="2">DATEDIF(TODAY(),L37,"y")&amp;"年"&amp;DATEDIF(TODAY(),L37,"ym")&amp;"月"</f>
-        <v>1年8月</v>
+        <v>1年6月</v>
       </c>
       <c r="N37" s="13"/>
-      <c r="O37" s="23"/>
+      <c r="O37" s="27"/>
       <c r="P37" s="12">
         <f>SUM(B38:O38)</f>
         <v>6</v>
@@ -3374,13 +3422,13 @@
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="25"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="29"/>
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
       <c r="N38" s="13"/>
-      <c r="O38" s="25"/>
+      <c r="O38" s="29"/>
       <c r="P38" s="12"/>
     </row>
     <row r="39" ht="36" customHeight="1" spans="1:16">
@@ -3414,16 +3462,16 @@
       <c r="J39" s="13">
         <v>5.207</v>
       </c>
-      <c r="K39" s="23"/>
-      <c r="L39" s="24">
+      <c r="K39" s="27"/>
+      <c r="L39" s="28">
         <v>46640</v>
       </c>
       <c r="M39" s="13" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>2年10月</v>
+        <v>2年8月</v>
       </c>
       <c r="N39" s="13"/>
-      <c r="O39" s="23"/>
+      <c r="O39" s="27"/>
       <c r="P39" s="12">
         <f>SUM(B40:O40)</f>
         <v>5</v>
@@ -3448,91 +3496,91 @@
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="25"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="29"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
       <c r="N40" s="13"/>
-      <c r="O40" s="25"/>
+      <c r="O40" s="29"/>
       <c r="P40" s="12"/>
     </row>
     <row r="41" ht="36" customHeight="1" spans="1:16">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="16">
         <v>5.9</v>
       </c>
-      <c r="G41" s="13" t="s">
+      <c r="G41" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H41" s="13">
+      <c r="H41" s="16">
         <v>-28.0231</v>
       </c>
-      <c r="I41" s="13">
+      <c r="I41" s="16">
         <v>19.8778</v>
       </c>
-      <c r="J41" s="13">
+      <c r="J41" s="16">
         <v>7.876</v>
       </c>
-      <c r="K41" s="23"/>
-      <c r="L41" s="24">
+      <c r="K41" s="35"/>
+      <c r="L41" s="36">
         <v>46129</v>
       </c>
-      <c r="M41" s="13" t="str">
+      <c r="M41" s="16" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>1年5月</v>
-      </c>
-      <c r="N41" s="13" t="s">
+        <v>1年3月</v>
+      </c>
+      <c r="N41" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="O41" s="23"/>
+      <c r="O41" s="35"/>
       <c r="P41" s="12">
         <f>SUM(B42:O42)</f>
         <v>9</v>
       </c>
     </row>
     <row r="42" ht="38" customHeight="1" spans="1:16">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13">
-        <v>1</v>
-      </c>
-      <c r="C42" s="13">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16">
+        <v>1</v>
+      </c>
+      <c r="C42" s="16">
         <v>0</v>
       </c>
-      <c r="D42" s="13">
-        <v>1</v>
-      </c>
-      <c r="E42" s="13">
-        <v>1</v>
-      </c>
-      <c r="F42" s="13">
+      <c r="D42" s="16">
+        <v>1</v>
+      </c>
+      <c r="E42" s="16">
+        <v>1</v>
+      </c>
+      <c r="F42" s="16">
         <v>5</v>
       </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13">
-        <v>1</v>
-      </c>
-      <c r="O42" s="25"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16">
+        <v>1</v>
+      </c>
+      <c r="O42" s="37"/>
       <c r="P42" s="12"/>
     </row>
     <row r="43" ht="36" customHeight="1" spans="1:16">
@@ -3556,11 +3604,11 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
-      <c r="K43" s="21"/>
+      <c r="K43" s="25"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
       <c r="N43" s="12"/>
-      <c r="O43" s="21"/>
+      <c r="O43" s="25"/>
       <c r="P43" s="12">
         <f>SUM(B44:O44)</f>
         <v>5</v>
@@ -3583,13 +3631,13 @@
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="31"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="38"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
-      <c r="N44" s="21"/>
-      <c r="O44" s="31"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="38"/>
       <c r="P44" s="12"/>
     </row>
     <row r="45" ht="36" hidden="1" customHeight="1" spans="1:16">
@@ -3613,11 +3661,11 @@
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
-      <c r="K45" s="21"/>
+      <c r="K45" s="25"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
-      <c r="O45" s="21"/>
+      <c r="O45" s="25"/>
       <c r="P45" s="12">
         <f t="shared" ref="P45:P49" si="3">SUM(B46:O46)</f>
         <v>4</v>
@@ -3640,41 +3688,41 @@
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="31"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="38"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
-      <c r="N46" s="21"/>
-      <c r="O46" s="31"/>
+      <c r="N46" s="25"/>
+      <c r="O46" s="38"/>
       <c r="P46" s="12"/>
     </row>
     <row r="47" ht="36" customHeight="1" spans="1:16">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12" t="s">
+      <c r="D47" s="18"/>
+      <c r="E47" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="12">
+      <c r="F47" s="18">
         <v>3</v>
       </c>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="21" t="s">
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="43" t="s">
         <v>62</v>
       </c>
       <c r="P47" s="12">
@@ -3683,29 +3731,29 @@
       </c>
     </row>
     <row r="48" ht="38" customHeight="1" spans="1:16">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18">
         <v>0</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C48" s="18">
         <v>0</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12">
-        <v>1</v>
-      </c>
-      <c r="F48" s="12">
+      <c r="D48" s="18"/>
+      <c r="E48" s="18">
+        <v>1</v>
+      </c>
+      <c r="F48" s="18">
         <v>3</v>
       </c>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="21"/>
-      <c r="O48" s="21">
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="43"/>
+      <c r="O48" s="43">
         <v>-1</v>
       </c>
       <c r="P48" s="12"/>
@@ -3733,11 +3781,11 @@
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="33"/>
-      <c r="N49" s="33"/>
-      <c r="O49" s="34"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="45"/>
+      <c r="M49" s="45"/>
+      <c r="N49" s="45"/>
+      <c r="O49" s="46"/>
       <c r="P49" s="12">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -3764,86 +3812,830 @@
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="33"/>
-      <c r="M50" s="33"/>
-      <c r="N50" s="33"/>
-      <c r="O50" s="34"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="45"/>
+      <c r="N50" s="45"/>
+      <c r="O50" s="46"/>
       <c r="P50" s="12"/>
     </row>
-    <row r="51" s="2" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A51" s="16" t="s">
+    <row r="51" s="2" customFormat="1" ht="36" customHeight="1" spans="1:388">
+      <c r="A51" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="F51" s="16">
+      <c r="F51" s="19">
         <v>3.4</v>
       </c>
-      <c r="G51" s="16" t="s">
+      <c r="G51" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H51" s="16">
+      <c r="H51" s="19">
         <v>-2.8973</v>
       </c>
-      <c r="I51" s="16">
+      <c r="I51" s="19">
         <v>37.1783</v>
       </c>
-      <c r="J51" s="16">
+      <c r="J51" s="19">
         <v>15.348</v>
       </c>
-      <c r="K51" s="35"/>
-      <c r="L51" s="36">
+      <c r="K51" s="47"/>
+      <c r="L51" s="48">
         <v>46401</v>
       </c>
-      <c r="M51" s="16" t="str">
+      <c r="M51" s="19" t="str">
         <f ca="1">DATEDIF(TODAY(),L51,"y")&amp;"年"&amp;DATEDIF(TODAY(),L51,"ym")&amp;"月"</f>
-        <v>2年2月</v>
-      </c>
-      <c r="N51" s="16"/>
-      <c r="O51" s="35"/>
-      <c r="P51" s="16">
+        <v>2年0月</v>
+      </c>
+      <c r="N51" s="19"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="12">
         <f t="shared" ref="P51:P55" si="4">SUM(B52:O52)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="52" s="2" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16">
-        <v>1</v>
-      </c>
-      <c r="C52" s="16">
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+      <c r="X51"/>
+      <c r="Y51"/>
+      <c r="Z51"/>
+      <c r="AA51"/>
+      <c r="AB51"/>
+      <c r="AC51"/>
+      <c r="AD51"/>
+      <c r="AE51"/>
+      <c r="AF51"/>
+      <c r="AG51"/>
+      <c r="AH51"/>
+      <c r="AI51"/>
+      <c r="AJ51"/>
+      <c r="AK51"/>
+      <c r="AL51"/>
+      <c r="AM51"/>
+      <c r="AN51"/>
+      <c r="AO51"/>
+      <c r="AP51"/>
+      <c r="AQ51"/>
+      <c r="AR51"/>
+      <c r="AS51"/>
+      <c r="AT51"/>
+      <c r="AU51"/>
+      <c r="AV51"/>
+      <c r="AW51"/>
+      <c r="AX51"/>
+      <c r="AY51"/>
+      <c r="AZ51"/>
+      <c r="BA51"/>
+      <c r="BB51"/>
+      <c r="BC51"/>
+      <c r="BD51"/>
+      <c r="BE51"/>
+      <c r="BF51"/>
+      <c r="BG51"/>
+      <c r="BH51"/>
+      <c r="BI51"/>
+      <c r="BJ51"/>
+      <c r="BK51"/>
+      <c r="BL51"/>
+      <c r="BM51"/>
+      <c r="BN51"/>
+      <c r="BO51"/>
+      <c r="BP51"/>
+      <c r="BQ51"/>
+      <c r="BR51"/>
+      <c r="BS51"/>
+      <c r="BT51"/>
+      <c r="BU51"/>
+      <c r="BV51"/>
+      <c r="BW51"/>
+      <c r="BX51"/>
+      <c r="BY51"/>
+      <c r="BZ51"/>
+      <c r="CA51"/>
+      <c r="CB51"/>
+      <c r="CC51"/>
+      <c r="CD51"/>
+      <c r="CE51"/>
+      <c r="CF51"/>
+      <c r="CG51"/>
+      <c r="CH51"/>
+      <c r="CI51"/>
+      <c r="CJ51"/>
+      <c r="CK51"/>
+      <c r="CL51"/>
+      <c r="CM51"/>
+      <c r="CN51"/>
+      <c r="CO51"/>
+      <c r="CP51"/>
+      <c r="CQ51"/>
+      <c r="CR51"/>
+      <c r="CS51"/>
+      <c r="CT51"/>
+      <c r="CU51"/>
+      <c r="CV51"/>
+      <c r="CW51"/>
+      <c r="CX51"/>
+      <c r="CY51"/>
+      <c r="CZ51"/>
+      <c r="DA51"/>
+      <c r="DB51"/>
+      <c r="DC51"/>
+      <c r="DD51"/>
+      <c r="DE51"/>
+      <c r="DF51"/>
+      <c r="DG51"/>
+      <c r="DH51"/>
+      <c r="DI51"/>
+      <c r="DJ51"/>
+      <c r="DK51"/>
+      <c r="DL51"/>
+      <c r="DM51"/>
+      <c r="DN51"/>
+      <c r="DO51"/>
+      <c r="DP51"/>
+      <c r="DQ51"/>
+      <c r="DR51"/>
+      <c r="DS51"/>
+      <c r="DT51"/>
+      <c r="DU51"/>
+      <c r="DV51"/>
+      <c r="DW51"/>
+      <c r="DX51"/>
+      <c r="DY51"/>
+      <c r="DZ51"/>
+      <c r="EA51"/>
+      <c r="EB51"/>
+      <c r="EC51"/>
+      <c r="ED51"/>
+      <c r="EE51"/>
+      <c r="EF51"/>
+      <c r="EG51"/>
+      <c r="EH51"/>
+      <c r="EI51"/>
+      <c r="EJ51"/>
+      <c r="EK51"/>
+      <c r="EL51"/>
+      <c r="EM51"/>
+      <c r="EN51"/>
+      <c r="EO51"/>
+      <c r="EP51"/>
+      <c r="EQ51"/>
+      <c r="ER51"/>
+      <c r="ES51"/>
+      <c r="ET51"/>
+      <c r="EU51"/>
+      <c r="EV51"/>
+      <c r="EW51"/>
+      <c r="EX51"/>
+      <c r="EY51"/>
+      <c r="EZ51"/>
+      <c r="FA51"/>
+      <c r="FB51"/>
+      <c r="FC51"/>
+      <c r="FD51"/>
+      <c r="FE51"/>
+      <c r="FF51"/>
+      <c r="FG51"/>
+      <c r="FH51"/>
+      <c r="FI51"/>
+      <c r="FJ51"/>
+      <c r="FK51"/>
+      <c r="FL51"/>
+      <c r="FM51"/>
+      <c r="FN51"/>
+      <c r="FO51"/>
+      <c r="FP51"/>
+      <c r="FQ51"/>
+      <c r="FR51"/>
+      <c r="FS51"/>
+      <c r="FT51"/>
+      <c r="FU51"/>
+      <c r="FV51"/>
+      <c r="FW51"/>
+      <c r="FX51"/>
+      <c r="FY51"/>
+      <c r="FZ51"/>
+      <c r="GA51"/>
+      <c r="GB51"/>
+      <c r="GC51"/>
+      <c r="GD51"/>
+      <c r="GE51"/>
+      <c r="GF51"/>
+      <c r="GG51"/>
+      <c r="GH51"/>
+      <c r="GI51"/>
+      <c r="GJ51"/>
+      <c r="GK51"/>
+      <c r="GL51"/>
+      <c r="GM51"/>
+      <c r="GN51"/>
+      <c r="GO51"/>
+      <c r="GP51"/>
+      <c r="GQ51"/>
+      <c r="GR51"/>
+      <c r="GS51"/>
+      <c r="GT51"/>
+      <c r="GU51"/>
+      <c r="GV51"/>
+      <c r="GW51"/>
+      <c r="GX51"/>
+      <c r="GY51"/>
+      <c r="GZ51"/>
+      <c r="HA51"/>
+      <c r="HB51"/>
+      <c r="HC51"/>
+      <c r="HD51"/>
+      <c r="HE51"/>
+      <c r="HF51"/>
+      <c r="HG51"/>
+      <c r="HH51"/>
+      <c r="HI51"/>
+      <c r="HJ51"/>
+      <c r="HK51"/>
+      <c r="HL51"/>
+      <c r="HM51"/>
+      <c r="HN51"/>
+      <c r="HO51"/>
+      <c r="HP51"/>
+      <c r="HQ51"/>
+      <c r="HR51"/>
+      <c r="HS51"/>
+      <c r="HT51"/>
+      <c r="HU51"/>
+      <c r="HV51"/>
+      <c r="HW51"/>
+      <c r="HX51"/>
+      <c r="HY51"/>
+      <c r="HZ51"/>
+      <c r="IA51"/>
+      <c r="IB51"/>
+      <c r="IC51"/>
+      <c r="ID51"/>
+      <c r="IE51"/>
+      <c r="IF51"/>
+      <c r="IG51"/>
+      <c r="IH51"/>
+      <c r="II51"/>
+      <c r="IJ51"/>
+      <c r="IK51"/>
+      <c r="IL51"/>
+      <c r="IM51"/>
+      <c r="IN51"/>
+      <c r="IO51"/>
+      <c r="IP51"/>
+      <c r="IQ51"/>
+      <c r="IR51"/>
+      <c r="IS51"/>
+      <c r="IT51"/>
+      <c r="IU51"/>
+      <c r="IV51"/>
+      <c r="IW51"/>
+      <c r="IX51"/>
+      <c r="IY51"/>
+      <c r="IZ51"/>
+      <c r="JA51"/>
+      <c r="JB51"/>
+      <c r="JC51"/>
+      <c r="JD51"/>
+      <c r="JE51"/>
+      <c r="JF51"/>
+      <c r="JG51"/>
+      <c r="JH51"/>
+      <c r="JI51"/>
+      <c r="JJ51"/>
+      <c r="JK51"/>
+      <c r="JL51"/>
+      <c r="JM51"/>
+      <c r="JN51"/>
+      <c r="JO51"/>
+      <c r="JP51"/>
+      <c r="JQ51"/>
+      <c r="JR51"/>
+      <c r="JS51"/>
+      <c r="JT51"/>
+      <c r="JU51"/>
+      <c r="JV51"/>
+      <c r="JW51"/>
+      <c r="JX51"/>
+      <c r="JY51"/>
+      <c r="JZ51"/>
+      <c r="KA51"/>
+      <c r="KB51"/>
+      <c r="KC51"/>
+      <c r="KD51"/>
+      <c r="KE51"/>
+      <c r="KF51"/>
+      <c r="KG51"/>
+      <c r="KH51"/>
+      <c r="KI51"/>
+      <c r="KJ51"/>
+      <c r="KK51"/>
+      <c r="KL51"/>
+      <c r="KM51"/>
+      <c r="KN51"/>
+      <c r="KO51"/>
+      <c r="KP51"/>
+      <c r="KQ51"/>
+      <c r="KR51"/>
+      <c r="KS51"/>
+      <c r="KT51"/>
+      <c r="KU51"/>
+      <c r="KV51"/>
+      <c r="KW51"/>
+      <c r="KX51"/>
+      <c r="KY51"/>
+      <c r="KZ51"/>
+      <c r="LA51"/>
+      <c r="LB51"/>
+      <c r="LC51"/>
+      <c r="LD51"/>
+      <c r="LE51"/>
+      <c r="LF51"/>
+      <c r="LG51"/>
+      <c r="LH51"/>
+      <c r="LI51"/>
+      <c r="LJ51"/>
+      <c r="LK51"/>
+      <c r="LL51"/>
+      <c r="LM51"/>
+      <c r="LN51"/>
+      <c r="LO51"/>
+      <c r="LP51"/>
+      <c r="LQ51"/>
+      <c r="LR51"/>
+      <c r="LS51"/>
+      <c r="LT51"/>
+      <c r="LU51"/>
+      <c r="LV51"/>
+      <c r="LW51"/>
+      <c r="LX51"/>
+      <c r="LY51"/>
+      <c r="LZ51"/>
+      <c r="MA51"/>
+      <c r="MB51"/>
+      <c r="MC51"/>
+      <c r="MD51"/>
+      <c r="ME51"/>
+      <c r="MF51"/>
+      <c r="MG51"/>
+      <c r="MH51"/>
+      <c r="MI51"/>
+      <c r="MJ51"/>
+      <c r="MK51"/>
+      <c r="ML51"/>
+      <c r="MM51"/>
+      <c r="MN51"/>
+      <c r="MO51"/>
+      <c r="MP51"/>
+      <c r="MQ51"/>
+      <c r="MR51"/>
+      <c r="MS51"/>
+      <c r="MT51"/>
+      <c r="MU51"/>
+      <c r="MV51"/>
+      <c r="MW51"/>
+      <c r="MX51"/>
+      <c r="MY51"/>
+      <c r="MZ51"/>
+      <c r="NA51"/>
+      <c r="NB51"/>
+      <c r="NC51"/>
+      <c r="ND51"/>
+      <c r="NE51"/>
+      <c r="NF51"/>
+      <c r="NG51"/>
+      <c r="NH51"/>
+      <c r="NI51"/>
+      <c r="NJ51"/>
+      <c r="NK51"/>
+      <c r="NL51"/>
+      <c r="NM51"/>
+      <c r="NN51"/>
+      <c r="NO51"/>
+      <c r="NP51"/>
+      <c r="NQ51"/>
+      <c r="NR51"/>
+      <c r="NS51"/>
+      <c r="NT51"/>
+      <c r="NU51"/>
+      <c r="NV51"/>
+      <c r="NW51"/>
+      <c r="NX51"/>
+    </row>
+    <row r="52" s="2" customFormat="1" ht="36" customHeight="1" spans="1:388">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19">
+        <v>1</v>
+      </c>
+      <c r="C52" s="19">
         <v>0</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="19">
         <v>0</v>
       </c>
-      <c r="E52" s="16">
-        <v>1</v>
-      </c>
-      <c r="F52" s="16">
+      <c r="E52" s="19">
+        <v>1</v>
+      </c>
+      <c r="F52" s="19">
         <v>3</v>
       </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="16"/>
-      <c r="M52" s="16"/>
-      <c r="N52" s="16"/>
-      <c r="O52" s="35"/>
-      <c r="P52" s="16"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="47"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="47"/>
+      <c r="P52" s="12"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
+      <c r="AA52"/>
+      <c r="AB52"/>
+      <c r="AC52"/>
+      <c r="AD52"/>
+      <c r="AE52"/>
+      <c r="AF52"/>
+      <c r="AG52"/>
+      <c r="AH52"/>
+      <c r="AI52"/>
+      <c r="AJ52"/>
+      <c r="AK52"/>
+      <c r="AL52"/>
+      <c r="AM52"/>
+      <c r="AN52"/>
+      <c r="AO52"/>
+      <c r="AP52"/>
+      <c r="AQ52"/>
+      <c r="AR52"/>
+      <c r="AS52"/>
+      <c r="AT52"/>
+      <c r="AU52"/>
+      <c r="AV52"/>
+      <c r="AW52"/>
+      <c r="AX52"/>
+      <c r="AY52"/>
+      <c r="AZ52"/>
+      <c r="BA52"/>
+      <c r="BB52"/>
+      <c r="BC52"/>
+      <c r="BD52"/>
+      <c r="BE52"/>
+      <c r="BF52"/>
+      <c r="BG52"/>
+      <c r="BH52"/>
+      <c r="BI52"/>
+      <c r="BJ52"/>
+      <c r="BK52"/>
+      <c r="BL52"/>
+      <c r="BM52"/>
+      <c r="BN52"/>
+      <c r="BO52"/>
+      <c r="BP52"/>
+      <c r="BQ52"/>
+      <c r="BR52"/>
+      <c r="BS52"/>
+      <c r="BT52"/>
+      <c r="BU52"/>
+      <c r="BV52"/>
+      <c r="BW52"/>
+      <c r="BX52"/>
+      <c r="BY52"/>
+      <c r="BZ52"/>
+      <c r="CA52"/>
+      <c r="CB52"/>
+      <c r="CC52"/>
+      <c r="CD52"/>
+      <c r="CE52"/>
+      <c r="CF52"/>
+      <c r="CG52"/>
+      <c r="CH52"/>
+      <c r="CI52"/>
+      <c r="CJ52"/>
+      <c r="CK52"/>
+      <c r="CL52"/>
+      <c r="CM52"/>
+      <c r="CN52"/>
+      <c r="CO52"/>
+      <c r="CP52"/>
+      <c r="CQ52"/>
+      <c r="CR52"/>
+      <c r="CS52"/>
+      <c r="CT52"/>
+      <c r="CU52"/>
+      <c r="CV52"/>
+      <c r="CW52"/>
+      <c r="CX52"/>
+      <c r="CY52"/>
+      <c r="CZ52"/>
+      <c r="DA52"/>
+      <c r="DB52"/>
+      <c r="DC52"/>
+      <c r="DD52"/>
+      <c r="DE52"/>
+      <c r="DF52"/>
+      <c r="DG52"/>
+      <c r="DH52"/>
+      <c r="DI52"/>
+      <c r="DJ52"/>
+      <c r="DK52"/>
+      <c r="DL52"/>
+      <c r="DM52"/>
+      <c r="DN52"/>
+      <c r="DO52"/>
+      <c r="DP52"/>
+      <c r="DQ52"/>
+      <c r="DR52"/>
+      <c r="DS52"/>
+      <c r="DT52"/>
+      <c r="DU52"/>
+      <c r="DV52"/>
+      <c r="DW52"/>
+      <c r="DX52"/>
+      <c r="DY52"/>
+      <c r="DZ52"/>
+      <c r="EA52"/>
+      <c r="EB52"/>
+      <c r="EC52"/>
+      <c r="ED52"/>
+      <c r="EE52"/>
+      <c r="EF52"/>
+      <c r="EG52"/>
+      <c r="EH52"/>
+      <c r="EI52"/>
+      <c r="EJ52"/>
+      <c r="EK52"/>
+      <c r="EL52"/>
+      <c r="EM52"/>
+      <c r="EN52"/>
+      <c r="EO52"/>
+      <c r="EP52"/>
+      <c r="EQ52"/>
+      <c r="ER52"/>
+      <c r="ES52"/>
+      <c r="ET52"/>
+      <c r="EU52"/>
+      <c r="EV52"/>
+      <c r="EW52"/>
+      <c r="EX52"/>
+      <c r="EY52"/>
+      <c r="EZ52"/>
+      <c r="FA52"/>
+      <c r="FB52"/>
+      <c r="FC52"/>
+      <c r="FD52"/>
+      <c r="FE52"/>
+      <c r="FF52"/>
+      <c r="FG52"/>
+      <c r="FH52"/>
+      <c r="FI52"/>
+      <c r="FJ52"/>
+      <c r="FK52"/>
+      <c r="FL52"/>
+      <c r="FM52"/>
+      <c r="FN52"/>
+      <c r="FO52"/>
+      <c r="FP52"/>
+      <c r="FQ52"/>
+      <c r="FR52"/>
+      <c r="FS52"/>
+      <c r="FT52"/>
+      <c r="FU52"/>
+      <c r="FV52"/>
+      <c r="FW52"/>
+      <c r="FX52"/>
+      <c r="FY52"/>
+      <c r="FZ52"/>
+      <c r="GA52"/>
+      <c r="GB52"/>
+      <c r="GC52"/>
+      <c r="GD52"/>
+      <c r="GE52"/>
+      <c r="GF52"/>
+      <c r="GG52"/>
+      <c r="GH52"/>
+      <c r="GI52"/>
+      <c r="GJ52"/>
+      <c r="GK52"/>
+      <c r="GL52"/>
+      <c r="GM52"/>
+      <c r="GN52"/>
+      <c r="GO52"/>
+      <c r="GP52"/>
+      <c r="GQ52"/>
+      <c r="GR52"/>
+      <c r="GS52"/>
+      <c r="GT52"/>
+      <c r="GU52"/>
+      <c r="GV52"/>
+      <c r="GW52"/>
+      <c r="GX52"/>
+      <c r="GY52"/>
+      <c r="GZ52"/>
+      <c r="HA52"/>
+      <c r="HB52"/>
+      <c r="HC52"/>
+      <c r="HD52"/>
+      <c r="HE52"/>
+      <c r="HF52"/>
+      <c r="HG52"/>
+      <c r="HH52"/>
+      <c r="HI52"/>
+      <c r="HJ52"/>
+      <c r="HK52"/>
+      <c r="HL52"/>
+      <c r="HM52"/>
+      <c r="HN52"/>
+      <c r="HO52"/>
+      <c r="HP52"/>
+      <c r="HQ52"/>
+      <c r="HR52"/>
+      <c r="HS52"/>
+      <c r="HT52"/>
+      <c r="HU52"/>
+      <c r="HV52"/>
+      <c r="HW52"/>
+      <c r="HX52"/>
+      <c r="HY52"/>
+      <c r="HZ52"/>
+      <c r="IA52"/>
+      <c r="IB52"/>
+      <c r="IC52"/>
+      <c r="ID52"/>
+      <c r="IE52"/>
+      <c r="IF52"/>
+      <c r="IG52"/>
+      <c r="IH52"/>
+      <c r="II52"/>
+      <c r="IJ52"/>
+      <c r="IK52"/>
+      <c r="IL52"/>
+      <c r="IM52"/>
+      <c r="IN52"/>
+      <c r="IO52"/>
+      <c r="IP52"/>
+      <c r="IQ52"/>
+      <c r="IR52"/>
+      <c r="IS52"/>
+      <c r="IT52"/>
+      <c r="IU52"/>
+      <c r="IV52"/>
+      <c r="IW52"/>
+      <c r="IX52"/>
+      <c r="IY52"/>
+      <c r="IZ52"/>
+      <c r="JA52"/>
+      <c r="JB52"/>
+      <c r="JC52"/>
+      <c r="JD52"/>
+      <c r="JE52"/>
+      <c r="JF52"/>
+      <c r="JG52"/>
+      <c r="JH52"/>
+      <c r="JI52"/>
+      <c r="JJ52"/>
+      <c r="JK52"/>
+      <c r="JL52"/>
+      <c r="JM52"/>
+      <c r="JN52"/>
+      <c r="JO52"/>
+      <c r="JP52"/>
+      <c r="JQ52"/>
+      <c r="JR52"/>
+      <c r="JS52"/>
+      <c r="JT52"/>
+      <c r="JU52"/>
+      <c r="JV52"/>
+      <c r="JW52"/>
+      <c r="JX52"/>
+      <c r="JY52"/>
+      <c r="JZ52"/>
+      <c r="KA52"/>
+      <c r="KB52"/>
+      <c r="KC52"/>
+      <c r="KD52"/>
+      <c r="KE52"/>
+      <c r="KF52"/>
+      <c r="KG52"/>
+      <c r="KH52"/>
+      <c r="KI52"/>
+      <c r="KJ52"/>
+      <c r="KK52"/>
+      <c r="KL52"/>
+      <c r="KM52"/>
+      <c r="KN52"/>
+      <c r="KO52"/>
+      <c r="KP52"/>
+      <c r="KQ52"/>
+      <c r="KR52"/>
+      <c r="KS52"/>
+      <c r="KT52"/>
+      <c r="KU52"/>
+      <c r="KV52"/>
+      <c r="KW52"/>
+      <c r="KX52"/>
+      <c r="KY52"/>
+      <c r="KZ52"/>
+      <c r="LA52"/>
+      <c r="LB52"/>
+      <c r="LC52"/>
+      <c r="LD52"/>
+      <c r="LE52"/>
+      <c r="LF52"/>
+      <c r="LG52"/>
+      <c r="LH52"/>
+      <c r="LI52"/>
+      <c r="LJ52"/>
+      <c r="LK52"/>
+      <c r="LL52"/>
+      <c r="LM52"/>
+      <c r="LN52"/>
+      <c r="LO52"/>
+      <c r="LP52"/>
+      <c r="LQ52"/>
+      <c r="LR52"/>
+      <c r="LS52"/>
+      <c r="LT52"/>
+      <c r="LU52"/>
+      <c r="LV52"/>
+      <c r="LW52"/>
+      <c r="LX52"/>
+      <c r="LY52"/>
+      <c r="LZ52"/>
+      <c r="MA52"/>
+      <c r="MB52"/>
+      <c r="MC52"/>
+      <c r="MD52"/>
+      <c r="ME52"/>
+      <c r="MF52"/>
+      <c r="MG52"/>
+      <c r="MH52"/>
+      <c r="MI52"/>
+      <c r="MJ52"/>
+      <c r="MK52"/>
+      <c r="ML52"/>
+      <c r="MM52"/>
+      <c r="MN52"/>
+      <c r="MO52"/>
+      <c r="MP52"/>
+      <c r="MQ52"/>
+      <c r="MR52"/>
+      <c r="MS52"/>
+      <c r="MT52"/>
+      <c r="MU52"/>
+      <c r="MV52"/>
+      <c r="MW52"/>
+      <c r="MX52"/>
+      <c r="MY52"/>
+      <c r="MZ52"/>
+      <c r="NA52"/>
+      <c r="NB52"/>
+      <c r="NC52"/>
+      <c r="ND52"/>
+      <c r="NE52"/>
+      <c r="NF52"/>
+      <c r="NG52"/>
+      <c r="NH52"/>
+      <c r="NI52"/>
+      <c r="NJ52"/>
+      <c r="NK52"/>
+      <c r="NL52"/>
+      <c r="NM52"/>
+      <c r="NN52"/>
+      <c r="NO52"/>
+      <c r="NP52"/>
+      <c r="NQ52"/>
+      <c r="NR52"/>
+      <c r="NS52"/>
+      <c r="NT52"/>
+      <c r="NU52"/>
+      <c r="NV52"/>
+      <c r="NW52"/>
+      <c r="NX52"/>
     </row>
     <row r="53" customFormat="1" ht="36" customHeight="1" spans="1:16">
       <c r="A53" s="12" t="s">
@@ -3876,16 +4668,16 @@
       <c r="J53" s="12">
         <v>2.117</v>
       </c>
-      <c r="K53" s="21"/>
-      <c r="L53" s="33" t="s">
+      <c r="K53" s="25"/>
+      <c r="L53" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="M53" s="33" t="str">
+      <c r="M53" s="45" t="str">
         <f ca="1">DATEDIF(TODAY(),L53,"y")&amp;"年"&amp;DATEDIF(TODAY(),L53,"ym")&amp;"月"</f>
-        <v>3年8月</v>
-      </c>
-      <c r="N53" s="33"/>
-      <c r="O53" s="34"/>
+        <v>3年6月</v>
+      </c>
+      <c r="N53" s="45"/>
+      <c r="O53" s="46"/>
       <c r="P53" s="12">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -3912,11 +4704,11 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
-      <c r="O54" s="34"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="45"/>
+      <c r="M54" s="45"/>
+      <c r="N54" s="45"/>
+      <c r="O54" s="46"/>
       <c r="P54" s="12"/>
     </row>
     <row r="55" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -3938,11 +4730,11 @@
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="33"/>
-      <c r="N55" s="33"/>
-      <c r="O55" s="34"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="45"/>
+      <c r="M55" s="45"/>
+      <c r="N55" s="45"/>
+      <c r="O55" s="46"/>
       <c r="P55" s="12">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -3965,11 +4757,11 @@
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="33"/>
-      <c r="N56" s="33"/>
-      <c r="O56" s="34"/>
+      <c r="K56" s="25"/>
+      <c r="L56" s="45"/>
+      <c r="M56" s="45"/>
+      <c r="N56" s="45"/>
+      <c r="O56" s="46"/>
       <c r="P56" s="12"/>
     </row>
     <row r="57" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -3993,11 +4785,11 @@
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="34"/>
+      <c r="K57" s="25"/>
+      <c r="L57" s="45"/>
+      <c r="M57" s="45"/>
+      <c r="N57" s="45"/>
+      <c r="O57" s="46"/>
       <c r="P57" s="12">
         <f t="shared" ref="P57:P61" si="5">SUM(B58:O58)</f>
         <v>4</v>
@@ -4022,11 +4814,11 @@
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33"/>
-      <c r="O58" s="34"/>
+      <c r="K58" s="25"/>
+      <c r="L58" s="45"/>
+      <c r="M58" s="45"/>
+      <c r="N58" s="45"/>
+      <c r="O58" s="46"/>
       <c r="P58" s="12"/>
     </row>
     <row r="59" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4052,11 +4844,11 @@
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33"/>
-      <c r="O59" s="34"/>
+      <c r="K59" s="25"/>
+      <c r="L59" s="45"/>
+      <c r="M59" s="45"/>
+      <c r="N59" s="45"/>
+      <c r="O59" s="46"/>
       <c r="P59" s="12">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -4083,11 +4875,11 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="33"/>
-      <c r="O60" s="34"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="45"/>
+      <c r="M60" s="45"/>
+      <c r="N60" s="45"/>
+      <c r="O60" s="46"/>
       <c r="P60" s="12"/>
     </row>
     <row r="61" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4113,11 +4905,11 @@
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="33"/>
-      <c r="N61" s="33"/>
-      <c r="O61" s="34"/>
+      <c r="K61" s="25"/>
+      <c r="L61" s="45"/>
+      <c r="M61" s="45"/>
+      <c r="N61" s="45"/>
+      <c r="O61" s="46"/>
       <c r="P61" s="12">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -4144,226 +4936,226 @@
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
-      <c r="O62" s="34"/>
+      <c r="K62" s="25"/>
+      <c r="L62" s="45"/>
+      <c r="M62" s="45"/>
+      <c r="N62" s="45"/>
+      <c r="O62" s="46"/>
       <c r="P62" s="12"/>
     </row>
     <row r="63" s="1" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="13" t="s">
+      <c r="E63" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F63" s="20">
         <v>3.4</v>
       </c>
-      <c r="G63" s="13" t="s">
+      <c r="G63" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="H63" s="13">
+      <c r="H63" s="20">
         <v>1.8781</v>
       </c>
-      <c r="I63" s="13">
+      <c r="I63" s="20">
         <v>81.9369</v>
       </c>
-      <c r="J63" s="13">
+      <c r="J63" s="20">
         <v>31.428</v>
       </c>
-      <c r="K63" s="23" t="s">
+      <c r="K63" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="L63" s="24">
+      <c r="L63" s="50">
         <v>46819</v>
       </c>
-      <c r="M63" s="13" t="str">
+      <c r="M63" s="20" t="str">
         <f ca="1">DATEDIF(TODAY(),L63,"y")&amp;"年"&amp;DATEDIF(TODAY(),L63,"ym")&amp;"月"</f>
-        <v>3年4月</v>
-      </c>
-      <c r="N63" s="13"/>
-      <c r="O63" s="23"/>
-      <c r="P63" s="13">
+        <v>3年2月</v>
+      </c>
+      <c r="N63" s="20"/>
+      <c r="O63" s="49"/>
+      <c r="P63" s="20">
         <f>SUM(B64:O64)</f>
         <v>6</v>
       </c>
     </row>
     <row r="64" s="1" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13">
-        <v>1</v>
-      </c>
-      <c r="C64" s="13">
+      <c r="A64" s="20"/>
+      <c r="B64" s="20">
+        <v>1</v>
+      </c>
+      <c r="C64" s="20">
         <v>0</v>
       </c>
-      <c r="D64" s="13">
-        <v>1</v>
-      </c>
-      <c r="E64" s="13">
-        <v>1</v>
-      </c>
-      <c r="F64" s="13">
+      <c r="D64" s="20">
+        <v>1</v>
+      </c>
+      <c r="E64" s="20">
+        <v>1</v>
+      </c>
+      <c r="F64" s="20">
         <v>3</v>
       </c>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="13"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="49"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="49"/>
+      <c r="P64" s="20"/>
     </row>
     <row r="65" s="3" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="B65" s="37" t="s">
+      <c r="B65" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="C65" s="37" t="s">
+      <c r="C65" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37" t="s">
+      <c r="D65" s="51"/>
+      <c r="E65" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="F65" s="37">
+      <c r="F65" s="51">
         <v>2.8</v>
       </c>
-      <c r="G65" s="37" t="s">
+      <c r="G65" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="H65" s="37">
+      <c r="H65" s="51">
         <v>-2.7335</v>
       </c>
-      <c r="I65" s="37">
+      <c r="I65" s="51">
         <v>28.3426</v>
       </c>
-      <c r="J65" s="37">
+      <c r="J65" s="51">
         <v>13.748</v>
       </c>
-      <c r="K65" s="38"/>
-      <c r="L65" s="39">
+      <c r="K65" s="52"/>
+      <c r="L65" s="53">
         <v>46234</v>
       </c>
-      <c r="M65" s="37" t="str">
+      <c r="M65" s="51" t="str">
         <f ca="1">DATEDIF(TODAY(),L65,"y")&amp;"年"&amp;DATEDIF(TODAY(),L65,"ym")&amp;"月"</f>
-        <v>1年9月</v>
-      </c>
-      <c r="N65" s="37"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="37">
+        <v>1年7月</v>
+      </c>
+      <c r="N65" s="51"/>
+      <c r="O65" s="52"/>
+      <c r="P65" s="51">
         <f>SUM(B66:O66)</f>
         <v>4</v>
       </c>
     </row>
     <row r="66" s="3" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A66" s="37"/>
-      <c r="B66" s="37">
-        <v>1</v>
-      </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37">
-        <v>1</v>
-      </c>
-      <c r="F66" s="37">
+      <c r="A66" s="51"/>
+      <c r="B66" s="51">
+        <v>1</v>
+      </c>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51">
+        <v>1</v>
+      </c>
+      <c r="F66" s="51">
         <v>2</v>
       </c>
-      <c r="G66" s="37"/>
-      <c r="H66" s="37"/>
-      <c r="I66" s="37"/>
-      <c r="J66" s="37"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="37"/>
-      <c r="M66" s="37"/>
-      <c r="N66" s="37"/>
-      <c r="O66" s="38"/>
-      <c r="P66" s="37"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="51"/>
+      <c r="M66" s="51"/>
+      <c r="N66" s="51"/>
+      <c r="O66" s="52"/>
+      <c r="P66" s="51"/>
     </row>
     <row r="67" s="3" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A67" s="37" t="s">
+      <c r="A67" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="B67" s="37" t="s">
+      <c r="B67" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="C67" s="37" t="s">
+      <c r="C67" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D67" s="37" t="s">
+      <c r="D67" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E67" s="37" t="s">
+      <c r="E67" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="F67" s="37">
+      <c r="F67" s="51">
         <v>2.5</v>
       </c>
-      <c r="G67" s="37" t="s">
+      <c r="G67" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="H67" s="37">
+      <c r="H67" s="51">
         <v>-28.102</v>
       </c>
-      <c r="I67" s="37">
+      <c r="I67" s="51">
         <v>105.8986</v>
       </c>
-      <c r="J67" s="37">
+      <c r="J67" s="51">
         <v>3.625</v>
       </c>
-      <c r="K67" s="38"/>
-      <c r="L67" s="39">
+      <c r="K67" s="52"/>
+      <c r="L67" s="53">
         <v>46218</v>
       </c>
-      <c r="M67" s="37" t="str">
+      <c r="M67" s="51" t="str">
         <f ca="1">DATEDIF(TODAY(),L67,"y")&amp;"年"&amp;DATEDIF(TODAY(),L67,"ym")&amp;"月"</f>
-        <v>1年8月</v>
-      </c>
-      <c r="N67" s="37"/>
-      <c r="O67" s="38"/>
-      <c r="P67" s="37">
+        <v>1年6月</v>
+      </c>
+      <c r="N67" s="51"/>
+      <c r="O67" s="52"/>
+      <c r="P67" s="51">
         <f>SUM(B68:O68)</f>
         <v>4</v>
       </c>
     </row>
     <row r="68" s="3" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37">
-        <v>1</v>
-      </c>
-      <c r="E68" s="37">
-        <v>1</v>
-      </c>
-      <c r="F68" s="37">
+      <c r="A68" s="51"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51">
+        <v>1</v>
+      </c>
+      <c r="E68" s="51">
+        <v>1</v>
+      </c>
+      <c r="F68" s="51">
         <v>2</v>
       </c>
-      <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
-      <c r="I68" s="37"/>
-      <c r="J68" s="37"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="37"/>
-      <c r="M68" s="37"/>
-      <c r="N68" s="37"/>
-      <c r="O68" s="38"/>
-      <c r="P68" s="37"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="51"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="52"/>
+      <c r="L68" s="51"/>
+      <c r="M68" s="51"/>
+      <c r="N68" s="51"/>
+      <c r="O68" s="52"/>
+      <c r="P68" s="51"/>
     </row>
     <row r="69" customFormat="1" ht="36" customHeight="1" spans="1:16">
       <c r="A69" s="12" t="s">
@@ -4384,16 +5176,16 @@
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="40">
+      <c r="K69" s="25"/>
+      <c r="L69" s="54">
         <v>46485</v>
       </c>
-      <c r="M69" s="33" t="str">
+      <c r="M69" s="45" t="str">
         <f ca="1">DATEDIF(TODAY(),L69,"y")&amp;"年"&amp;DATEDIF(TODAY(),L69,"ym")&amp;"月"</f>
-        <v>2年5月</v>
-      </c>
-      <c r="N69" s="33"/>
-      <c r="O69" s="34"/>
+        <v>2年3月</v>
+      </c>
+      <c r="N69" s="45"/>
+      <c r="O69" s="46"/>
       <c r="P69" s="12">
         <f t="shared" ref="P69:P73" si="6">SUM(B70:O70)</f>
         <v>4</v>
@@ -4416,11 +5208,11 @@
       <c r="H70" s="12"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
-      <c r="K70" s="21"/>
-      <c r="L70" s="33"/>
-      <c r="M70" s="33"/>
-      <c r="N70" s="33"/>
-      <c r="O70" s="34"/>
+      <c r="K70" s="25"/>
+      <c r="L70" s="45"/>
+      <c r="M70" s="45"/>
+      <c r="N70" s="45"/>
+      <c r="O70" s="46"/>
       <c r="P70" s="12"/>
     </row>
     <row r="71" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4442,11 +5234,11 @@
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
-      <c r="K71" s="21"/>
-      <c r="L71" s="33"/>
-      <c r="M71" s="33"/>
-      <c r="N71" s="33"/>
-      <c r="O71" s="34"/>
+      <c r="K71" s="25"/>
+      <c r="L71" s="45"/>
+      <c r="M71" s="45"/>
+      <c r="N71" s="45"/>
+      <c r="O71" s="46"/>
       <c r="P71" s="12">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -4469,11 +5261,11 @@
       <c r="H72" s="12"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
-      <c r="K72" s="21"/>
-      <c r="L72" s="33"/>
-      <c r="M72" s="33"/>
-      <c r="N72" s="33"/>
-      <c r="O72" s="34"/>
+      <c r="K72" s="25"/>
+      <c r="L72" s="45"/>
+      <c r="M72" s="45"/>
+      <c r="N72" s="45"/>
+      <c r="O72" s="46"/>
       <c r="P72" s="12"/>
     </row>
     <row r="73" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4505,16 +5297,16 @@
       <c r="J73" s="13">
         <v>3.865</v>
       </c>
-      <c r="K73" s="23"/>
-      <c r="L73" s="24">
+      <c r="K73" s="27"/>
+      <c r="L73" s="28">
         <v>46955</v>
       </c>
-      <c r="M73" s="23" t="str">
+      <c r="M73" s="27" t="str">
         <f ca="1" t="shared" ref="M73:M77" si="7">DATEDIF(TODAY(),L73,"y")&amp;"年"&amp;DATEDIF(TODAY(),L73,"ym")&amp;"月"</f>
-        <v>3年8月</v>
-      </c>
-      <c r="N73" s="23"/>
-      <c r="O73" s="23"/>
+        <v>3年6月</v>
+      </c>
+      <c r="N73" s="27"/>
+      <c r="O73" s="27"/>
       <c r="P73" s="12">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -4537,11 +5329,11 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="24"/>
-      <c r="M74" s="23"/>
-      <c r="N74" s="23"/>
-      <c r="O74" s="23"/>
+      <c r="K74" s="27"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="27"/>
+      <c r="N74" s="27"/>
+      <c r="O74" s="27"/>
       <c r="P74" s="12"/>
     </row>
     <row r="75" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4573,18 +5365,18 @@
       <c r="J75" s="13">
         <v>9.391</v>
       </c>
-      <c r="K75" s="23"/>
-      <c r="L75" s="24">
+      <c r="K75" s="27"/>
+      <c r="L75" s="28">
         <v>46220</v>
       </c>
-      <c r="M75" s="23" t="str">
+      <c r="M75" s="27" t="str">
         <f ca="1" t="shared" si="7"/>
-        <v>1年8月</v>
-      </c>
-      <c r="N75" s="23" t="s">
+        <v>1年6月</v>
+      </c>
+      <c r="N75" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="O75" s="23"/>
+      <c r="O75" s="27"/>
       <c r="P75" s="12">
         <f t="shared" ref="P75:P79" si="8">SUM(B76:O76)</f>
         <v>5</v>
@@ -4607,13 +5399,13 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="24"/>
-      <c r="M76" s="23"/>
-      <c r="N76" s="23">
-        <v>1</v>
-      </c>
-      <c r="O76" s="23"/>
+      <c r="K76" s="27"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="27"/>
+      <c r="N76" s="27">
+        <v>1</v>
+      </c>
+      <c r="O76" s="27"/>
       <c r="P76" s="12"/>
     </row>
     <row r="77" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4645,18 +5437,18 @@
       <c r="J77" s="15">
         <v>2.889</v>
       </c>
-      <c r="K77" s="27" t="s">
+      <c r="K77" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="L77" s="28">
+      <c r="L77" s="32">
         <v>46371</v>
       </c>
-      <c r="M77" s="27" t="str">
+      <c r="M77" s="31" t="str">
         <f ca="1" t="shared" si="7"/>
-        <v>2年1月</v>
-      </c>
-      <c r="N77" s="27"/>
-      <c r="O77" s="27"/>
+        <v>1年11月</v>
+      </c>
+      <c r="N77" s="31"/>
+      <c r="O77" s="31"/>
       <c r="P77" s="12">
         <f t="shared" si="8"/>
         <v>3</v>
@@ -4679,13 +5471,13 @@
       <c r="H78" s="15"/>
       <c r="I78" s="15"/>
       <c r="J78" s="15"/>
-      <c r="K78" s="29">
+      <c r="K78" s="33">
         <v>-1</v>
       </c>
-      <c r="L78" s="28"/>
-      <c r="M78" s="27"/>
-      <c r="N78" s="27"/>
-      <c r="O78" s="27"/>
+      <c r="L78" s="32"/>
+      <c r="M78" s="31"/>
+      <c r="N78" s="31"/>
+      <c r="O78" s="31"/>
       <c r="P78" s="12"/>
     </row>
     <row r="79" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4717,18 +5509,18 @@
       <c r="J79" s="13">
         <v>20.253</v>
       </c>
-      <c r="K79" s="23" t="s">
+      <c r="K79" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="L79" s="24">
+      <c r="L79" s="28">
         <v>46017</v>
       </c>
-      <c r="M79" s="23" t="str">
+      <c r="M79" s="27" t="str">
         <f ca="1" t="shared" ref="M79:M83" si="9">DATEDIF(TODAY(),L79,"y")&amp;"年"&amp;DATEDIF(TODAY(),L79,"ym")&amp;"月"</f>
-        <v>1年1月</v>
-      </c>
-      <c r="N79" s="23"/>
-      <c r="O79" s="23"/>
+        <v>0年11月</v>
+      </c>
+      <c r="N79" s="27"/>
+      <c r="O79" s="27"/>
       <c r="P79" s="12">
         <f t="shared" si="8"/>
         <v>3</v>
@@ -4751,83 +5543,83 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
       <c r="J80" s="13"/>
-      <c r="K80" s="25"/>
-      <c r="L80" s="24"/>
-      <c r="M80" s="23"/>
-      <c r="N80" s="23"/>
-      <c r="O80" s="23"/>
+      <c r="K80" s="29"/>
+      <c r="L80" s="28"/>
+      <c r="M80" s="27"/>
+      <c r="N80" s="27"/>
+      <c r="O80" s="27"/>
       <c r="P80" s="12"/>
     </row>
     <row r="81" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13" t="s">
+      <c r="B81" s="16"/>
+      <c r="C81" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="D81" s="13" t="s">
+      <c r="D81" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="13" t="s">
+      <c r="E81" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="F81" s="13">
+      <c r="F81" s="16">
         <v>1.6</v>
       </c>
-      <c r="G81" s="13" t="s">
+      <c r="G81" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H81" s="13">
+      <c r="H81" s="16">
         <v>18.0689</v>
       </c>
-      <c r="I81" s="13">
+      <c r="I81" s="16">
         <v>48.4298</v>
       </c>
-      <c r="J81" s="13">
+      <c r="J81" s="16">
         <v>5.86</v>
       </c>
-      <c r="K81" s="23"/>
-      <c r="L81" s="24">
+      <c r="K81" s="35"/>
+      <c r="L81" s="36">
         <v>46371</v>
       </c>
-      <c r="M81" s="23" t="str">
+      <c r="M81" s="35" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>2年1月</v>
-      </c>
-      <c r="N81" s="23" t="s">
+        <v>1年11月</v>
+      </c>
+      <c r="N81" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="O81" s="23"/>
+      <c r="O81" s="35"/>
       <c r="P81" s="12">
         <f>SUM(B82:O82)</f>
         <v>4</v>
       </c>
     </row>
     <row r="82" customFormat="1" ht="36" customHeight="1" spans="1:16">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13">
-        <v>1</v>
-      </c>
-      <c r="E82" s="13">
-        <v>1</v>
-      </c>
-      <c r="F82" s="13">
-        <v>1</v>
-      </c>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="25"/>
-      <c r="L82" s="24"/>
-      <c r="M82" s="23"/>
-      <c r="N82" s="25">
-        <v>1</v>
-      </c>
-      <c r="O82" s="23"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16">
+        <v>1</v>
+      </c>
+      <c r="E82" s="16">
+        <v>1</v>
+      </c>
+      <c r="F82" s="16">
+        <v>1</v>
+      </c>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="37"/>
+      <c r="L82" s="36"/>
+      <c r="M82" s="35"/>
+      <c r="N82" s="37">
+        <v>1</v>
+      </c>
+      <c r="O82" s="35"/>
       <c r="P82" s="12"/>
     </row>
     <row r="83" customFormat="1" ht="36" customHeight="1" spans="1:16">
@@ -4859,16 +5651,16 @@
       <c r="J83" s="13">
         <v>5.548</v>
       </c>
-      <c r="K83" s="23"/>
-      <c r="L83" s="24">
+      <c r="K83" s="27"/>
+      <c r="L83" s="28">
         <v>46834</v>
       </c>
-      <c r="M83" s="23" t="str">
+      <c r="M83" s="27" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>3年4月</v>
-      </c>
-      <c r="N83" s="23"/>
-      <c r="O83" s="23"/>
+        <v>3年2月</v>
+      </c>
+      <c r="N83" s="27"/>
+      <c r="O83" s="27"/>
       <c r="P83" s="12">
         <f>SUM(B84:O84)</f>
         <v>5</v>
@@ -4891,11 +5683,11 @@
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
       <c r="J84" s="13"/>
-      <c r="K84" s="25"/>
-      <c r="L84" s="24"/>
-      <c r="M84" s="23"/>
-      <c r="N84" s="25"/>
-      <c r="O84" s="23"/>
+      <c r="K84" s="29"/>
+      <c r="L84" s="28"/>
+      <c r="M84" s="27"/>
+      <c r="N84" s="29"/>
+      <c r="O84" s="27"/>
       <c r="P84" s="12"/>
     </row>
   </sheetData>

</xml_diff>